<commit_message>
integration of filter area (need to generalize)
</commit_message>
<xml_diff>
--- a/Modules/Main/results.xlsx
+++ b/Modules/Main/results.xlsx
@@ -9,7 +9,7 @@
     <sheet name="result" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="0" fullCalcOnLoad="1"/>
+  <calcPr calcId="191029" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -424,10 +424,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D31"/>
+  <dimension ref="A1:D29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -445,6 +445,11 @@
       </c>
       <c r="C1" t="inlineStr">
         <is>
+          <t>total time [sec]</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
           <t>cpu total time [sec]</t>
         </is>
       </c>
@@ -473,255 +478,321 @@
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>39.78</v>
+        <v>39.06</v>
       </c>
       <c r="B4" t="n">
-        <v>0.16</v>
+        <v>0.04000000000000001</v>
       </c>
       <c r="C4" t="n">
-        <v>10.70983195304871</v>
+        <v>6.14512300491333</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>37.37</v>
+        <v>39.78</v>
       </c>
       <c r="B5" t="n">
-        <v>0.36</v>
+        <v>0.16</v>
       </c>
       <c r="C5" t="n">
-        <v>29.24841785430908</v>
+        <v>10.57961821556091</v>
+      </c>
+      <c r="D5" t="n">
+        <v>9.328125</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>43.48</v>
+        <v>39.78</v>
       </c>
       <c r="B6" t="n">
-        <v>1</v>
+        <v>0.16</v>
       </c>
       <c r="C6" t="n">
-        <v>65.27312445640564</v>
+        <v>13.87360000610352</v>
+      </c>
+      <c r="D6" t="n">
+        <v>12.53125</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>98.77</v>
+        <v>39.06</v>
       </c>
       <c r="B7" t="n">
-        <v>1</v>
+        <v>0.04000000000000001</v>
       </c>
       <c r="C7" t="n">
-        <v>135.7349853515625</v>
+        <v>3.679166555404663</v>
+      </c>
+      <c r="D7" t="n">
+        <v>2.453125</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>2.22</v>
+        <v>39.06</v>
       </c>
       <c r="B8" t="n">
         <v>0.04000000000000001</v>
       </c>
       <c r="C8" t="n">
-        <v>2.05316686630249</v>
+        <v>3.316033124923706</v>
+      </c>
+      <c r="D8" t="n">
+        <v>2.5625</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>28.99</v>
+        <v>39.06</v>
       </c>
       <c r="B9" t="n">
-        <v>1</v>
+        <v>0.04000000000000001</v>
       </c>
       <c r="C9" t="n">
-        <v>62.21622347831726</v>
+        <v>3.487463235855103</v>
+      </c>
+      <c r="D9" t="n">
+        <v>2.953125</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>23.34</v>
+        <v>39.06</v>
       </c>
       <c r="B10" t="n">
-        <v>0.16</v>
+        <v>0.04000000000000001</v>
       </c>
       <c r="C10" t="n">
-        <v>8.734398603439331</v>
+        <v>3.183549880981445</v>
+      </c>
+      <c r="D10" t="n">
+        <v>2.546875</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>99.67</v>
+        <v>39.78</v>
       </c>
       <c r="B11" t="n">
         <v>0.16</v>
       </c>
       <c r="C11" t="n">
-        <v>17.93797159194946</v>
+        <v>10.6967921257019</v>
+      </c>
+      <c r="D11" t="n">
+        <v>9.96875</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>87.66</v>
+        <v>39.78</v>
       </c>
       <c r="B12" t="n">
-        <v>1</v>
+        <v>0.16</v>
       </c>
       <c r="C12" t="n">
-        <v>106.0952725410461</v>
+        <v>10.07253766059875</v>
+      </c>
+      <c r="D12" t="n">
+        <v>9.359375</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>42.85</v>
+        <v>39.78</v>
       </c>
       <c r="B13" t="n">
-        <v>0.6400000000000001</v>
+        <v>0.16</v>
       </c>
       <c r="C13" t="n">
-        <v>53.67893099784851</v>
+        <v>12.94005417823792</v>
+      </c>
+      <c r="D13" t="n">
+        <v>12.25</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>29.49</v>
+        <v>39.06</v>
       </c>
       <c r="B14" t="n">
-        <v>1.44</v>
+        <v>0.04000000000000001</v>
       </c>
       <c r="C14" t="n">
-        <v>101.9017038345337</v>
+        <v>3.162457466125488</v>
+      </c>
+      <c r="D14" t="n">
+        <v>2.515625</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>28.93</v>
+        <v>39.06</v>
       </c>
       <c r="B15" t="n">
-        <v>1</v>
+        <v>0.04000000000000001</v>
       </c>
       <c r="C15" t="n">
-        <v>78.61512589454651</v>
+        <v>3.130092859268188</v>
+      </c>
+      <c r="D15" t="n">
+        <v>2.4375</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>12.05</v>
+        <v>39.06</v>
       </c>
       <c r="B16" t="n">
-        <v>1</v>
+        <v>0.04000000000000001</v>
       </c>
       <c r="C16" t="n">
-        <v>44.66143202781677</v>
+        <v>7.798795700073242</v>
+      </c>
+      <c r="D16" t="n">
+        <v>6.578125</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>11.31</v>
+        <v>39.06</v>
       </c>
       <c r="B17" t="n">
-        <v>1.96</v>
+        <v>0.04000000000000001</v>
       </c>
       <c r="C17" t="n">
-        <v>71.80608463287354</v>
+        <v>3.232581853866577</v>
+      </c>
+      <c r="D17" t="n">
+        <v>2.546875</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>20.3</v>
+        <v>39.06</v>
       </c>
       <c r="B18" t="n">
-        <v>1.44</v>
+        <v>0.04000000000000001</v>
       </c>
       <c r="C18" t="n">
-        <v>93.0687084197998</v>
+        <v>3.882983684539795</v>
+      </c>
+      <c r="D18" t="n">
+        <v>3.203125</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>23.59</v>
+        <v>39.06</v>
       </c>
       <c r="B19" t="n">
-        <v>0.36</v>
+        <v>0.04000000000000001</v>
       </c>
       <c r="C19" t="n">
-        <v>20.67740511894226</v>
+        <v>3.353356122970581</v>
+      </c>
+      <c r="D19" t="n">
+        <v>2.578125</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>15.92</v>
+        <v>39.06</v>
       </c>
       <c r="B20" t="n">
-        <v>1</v>
+        <v>0.04000000000000001</v>
       </c>
       <c r="C20" t="n">
-        <v>46.42787218093872</v>
+        <v>3.265630006790161</v>
+      </c>
+      <c r="D20" t="n">
+        <v>2.625</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>10.12</v>
+        <v>39.06</v>
       </c>
       <c r="B21" t="n">
-        <v>1</v>
+        <v>0.04000000000000001</v>
       </c>
       <c r="C21" t="n">
-        <v>33.45044231414795</v>
+        <v>3.232125759124756</v>
+      </c>
+      <c r="D21" t="n">
+        <v>2.4375</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>10.12</v>
+        <v>39.78</v>
       </c>
       <c r="B22" t="n">
-        <v>1</v>
+        <v>0.16</v>
       </c>
       <c r="C22" t="n">
-        <v>35.61816668510437</v>
+        <v>10.40235781669617</v>
+      </c>
+      <c r="D22" t="n">
+        <v>9.59375</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>36.19</v>
+        <v>39.78</v>
       </c>
       <c r="B23" t="n">
-        <v>2.56</v>
+        <v>0.16</v>
       </c>
       <c r="C23" t="n">
-        <v>216.7178537845612</v>
+        <v>12.70899796485901</v>
+      </c>
+      <c r="D23" t="n">
+        <v>11.65625</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>30.88</v>
+        <v>39.06</v>
       </c>
       <c r="B24" t="n">
-        <v>1</v>
+        <v>0.04000000000000001</v>
       </c>
       <c r="C24" t="n">
-        <v>76.06927084922791</v>
+        <v>3.043107748031616</v>
+      </c>
+      <c r="D24" t="n">
+        <v>2.4375</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>39.06</v>
+        <v>39.78</v>
       </c>
       <c r="B25" t="n">
-        <v>0.04000000000000001</v>
+        <v>0.16</v>
       </c>
       <c r="C25" t="n">
-        <v>8.133701801300049</v>
+        <v>9.73159646987915</v>
+      </c>
+      <c r="D25" t="n">
+        <v>9.046875</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>39.06</v>
+        <v>39.78</v>
       </c>
       <c r="B26" t="n">
-        <v>0.04000000000000001</v>
+        <v>0.16</v>
       </c>
       <c r="C26" t="n">
-        <v>8.123492240905762</v>
+        <v>14.91842198371887</v>
+      </c>
+      <c r="D26" t="n">
+        <v>12.90625</v>
       </c>
     </row>
     <row r="27">
@@ -732,18 +803,24 @@
         <v>0.16</v>
       </c>
       <c r="C27" t="n">
-        <v>21.38716721534729</v>
+        <v>35.30180263519287</v>
+      </c>
+      <c r="D27" t="n">
+        <v>19.0625</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>39.06</v>
+        <v>39.78</v>
       </c>
       <c r="B28" t="n">
-        <v>0.04000000000000001</v>
+        <v>0.16</v>
       </c>
       <c r="C28" t="n">
-        <v>8.581060886383057</v>
+        <v>12.96200776100159</v>
+      </c>
+      <c r="D28" t="n">
+        <v>11.984375</v>
       </c>
     </row>
     <row r="29">
@@ -754,32 +831,10 @@
         <v>0.16</v>
       </c>
       <c r="C29" t="n">
-        <v>23.72981786727905</v>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" t="n">
-        <v>39.06</v>
-      </c>
-      <c r="B30" t="n">
-        <v>0.04000000000000001</v>
-      </c>
-      <c r="C30" t="n">
-        <v>5.445710897445679</v>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" t="n">
-        <v>39.06</v>
-      </c>
-      <c r="B31" t="n">
-        <v>0.04000000000000001</v>
-      </c>
-      <c r="C31" t="n">
-        <v>4.061498165130615</v>
-      </c>
-      <c r="D31" t="n">
-        <v>3.328125</v>
+        <v>10.17955327033997</v>
+      </c>
+      <c r="D29" t="n">
+        <v>9.296875</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update progressbar now with slopy
</commit_message>
<xml_diff>
--- a/Modules/Main/results.xlsx
+++ b/Modules/Main/results.xlsx
@@ -3,13 +3,13 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="result" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="191029" fullCalcOnLoad="1"/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -424,13 +424,13 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D54"/>
+  <dimension ref="A1:D77"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="C65" sqref="C65"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1">
       <c r="A1" t="inlineStr">
@@ -1187,6 +1187,328 @@
         <v>20.1875</v>
       </c>
     </row>
+    <row r="55">
+      <c r="A55" t="n">
+        <v>37.37</v>
+      </c>
+      <c r="B55" t="n">
+        <v>0.36</v>
+      </c>
+      <c r="C55" t="n">
+        <v>20.14945220947266</v>
+      </c>
+      <c r="D55" t="n">
+        <v>19.46875</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="n">
+        <v>50.14</v>
+      </c>
+      <c r="B56" t="n">
+        <v>0.04000000000000001</v>
+      </c>
+      <c r="C56" t="n">
+        <v>3.571915864944458</v>
+      </c>
+      <c r="D56" t="n">
+        <v>2.828125</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="n">
+        <v>55.75</v>
+      </c>
+      <c r="B57" t="n">
+        <v>0.16</v>
+      </c>
+      <c r="C57" t="n">
+        <v>12.53389739990234</v>
+      </c>
+      <c r="D57" t="n">
+        <v>11.015625</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="n">
+        <v>32.28</v>
+      </c>
+      <c r="B58" t="n">
+        <v>0.16</v>
+      </c>
+      <c r="C58" t="n">
+        <v>9.142158031463623</v>
+      </c>
+      <c r="D58" t="n">
+        <v>7.828125</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="n">
+        <v>27.15</v>
+      </c>
+      <c r="B59" t="n">
+        <v>0.16</v>
+      </c>
+      <c r="C59" t="n">
+        <v>9.069642543792725</v>
+      </c>
+      <c r="D59" t="n">
+        <v>7.25</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="n">
+        <v>42.14</v>
+      </c>
+      <c r="B60" t="n">
+        <v>0.36</v>
+      </c>
+      <c r="C60" t="n">
+        <v>21.91850090026855</v>
+      </c>
+      <c r="D60" t="n">
+        <v>20.765625</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="n">
+        <v>42.14</v>
+      </c>
+      <c r="B61" t="n">
+        <v>0.36</v>
+      </c>
+      <c r="C61" t="n">
+        <v>26.33934664726257</v>
+      </c>
+      <c r="D61" t="n">
+        <v>25.609375</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="n">
+        <v>39.78</v>
+      </c>
+      <c r="B62" t="n">
+        <v>0.16</v>
+      </c>
+      <c r="C62" t="n">
+        <v>11.15482640266418</v>
+      </c>
+      <c r="D62" t="n">
+        <v>9.734375</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="n">
+        <v>100</v>
+      </c>
+      <c r="B63" t="n">
+        <v>0.16</v>
+      </c>
+      <c r="C63" t="n">
+        <v>36.07674241065979</v>
+      </c>
+      <c r="D63" t="n">
+        <v>31.859375</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="n">
+        <v>93.69</v>
+      </c>
+      <c r="B64" t="n">
+        <v>0.16</v>
+      </c>
+      <c r="C64" t="n">
+        <v>56.04600739479065</v>
+      </c>
+      <c r="D64" t="n">
+        <v>52.6875</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="n">
+        <v>98.48999999999999</v>
+      </c>
+      <c r="B65" t="n">
+        <v>0.16</v>
+      </c>
+      <c r="C65" t="n">
+        <v>51.7009365558624</v>
+      </c>
+      <c r="D65" t="n">
+        <v>49.421875</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="n">
+        <v>97.64</v>
+      </c>
+      <c r="B66" t="n">
+        <v>1</v>
+      </c>
+      <c r="C66" t="n">
+        <v>185.6703400611877</v>
+      </c>
+      <c r="D66" t="n">
+        <v>184.015625</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="n">
+        <v>39.78</v>
+      </c>
+      <c r="B67" t="n">
+        <v>0.16</v>
+      </c>
+      <c r="C67" t="n">
+        <v>17.71249747276306</v>
+      </c>
+      <c r="D67" t="n">
+        <v>15.78125</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="n">
+        <v>39.78</v>
+      </c>
+      <c r="B68" t="n">
+        <v>0.16</v>
+      </c>
+      <c r="C68" t="n">
+        <v>30.19679999351501</v>
+      </c>
+      <c r="D68" t="n">
+        <v>26.5625</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="n">
+        <v>39.78</v>
+      </c>
+      <c r="B69" t="n">
+        <v>0.16</v>
+      </c>
+      <c r="C69" t="n">
+        <v>22.50559282302856</v>
+      </c>
+      <c r="D69" t="n">
+        <v>22.046875</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="n">
+        <v>39.78</v>
+      </c>
+      <c r="B70" t="n">
+        <v>0.16</v>
+      </c>
+      <c r="C70" t="n">
+        <v>31.25962972640991</v>
+      </c>
+      <c r="D70" t="n">
+        <v>29.96875</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="n">
+        <v>39.78</v>
+      </c>
+      <c r="B71" t="n">
+        <v>0.16</v>
+      </c>
+      <c r="C71" t="n">
+        <v>20.78266620635986</v>
+      </c>
+      <c r="D71" t="n">
+        <v>19.890625</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="n">
+        <v>39.78</v>
+      </c>
+      <c r="B72" t="n">
+        <v>0.16</v>
+      </c>
+      <c r="C72" t="n">
+        <v>30.54809165000916</v>
+      </c>
+      <c r="D72" t="n">
+        <v>28.859375</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="n">
+        <v>39.78</v>
+      </c>
+      <c r="B73" t="n">
+        <v>0.16</v>
+      </c>
+      <c r="C73" t="n">
+        <v>10.35814690589905</v>
+      </c>
+      <c r="D73" t="n">
+        <v>9.109375</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="n">
+        <v>41.49</v>
+      </c>
+      <c r="B74" t="n">
+        <v>0.16</v>
+      </c>
+      <c r="C74" t="n">
+        <v>10.58113431930542</v>
+      </c>
+      <c r="D74" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="n">
+        <v>38.24</v>
+      </c>
+      <c r="B75" t="n">
+        <v>0.36</v>
+      </c>
+      <c r="C75" t="n">
+        <v>21.57353019714355</v>
+      </c>
+      <c r="D75" t="n">
+        <v>19.59375</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="n">
+        <v>28.18</v>
+      </c>
+      <c r="B76" t="n">
+        <v>0.36</v>
+      </c>
+      <c r="C76" t="n">
+        <v>26.47938179969788</v>
+      </c>
+      <c r="D76" t="n">
+        <v>23.5625</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="n">
+        <v>53.66</v>
+      </c>
+      <c r="B77" t="n">
+        <v>0.36</v>
+      </c>
+      <c r="C77" t="n">
+        <v>27.1538360118866</v>
+      </c>
+      <c r="D77" t="n">
+        <v>24.921875</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
improve runtime when calclate total mask
</commit_message>
<xml_diff>
--- a/Modules/Main/results.xlsx
+++ b/Modules/Main/results.xlsx
@@ -424,7 +424,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -551,6 +551,328 @@
         <v>2.171875</v>
       </c>
     </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>100</v>
+      </c>
+      <c r="B10" t="n">
+        <v>0.04000000000000001</v>
+      </c>
+      <c r="C10" t="n">
+        <v>6.683801412582397</v>
+      </c>
+      <c r="D10" t="n">
+        <v>6.015625</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>100</v>
+      </c>
+      <c r="B11" t="n">
+        <v>0.36</v>
+      </c>
+      <c r="C11" t="n">
+        <v>107.3484826087952</v>
+      </c>
+      <c r="D11" t="n">
+        <v>105.28125</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>100</v>
+      </c>
+      <c r="B12" t="n">
+        <v>0.04000000000000001</v>
+      </c>
+      <c r="C12" t="n">
+        <v>7.325151681900024</v>
+      </c>
+      <c r="D12" t="n">
+        <v>6.625</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>100</v>
+      </c>
+      <c r="B13" t="n">
+        <v>0.04000000000000001</v>
+      </c>
+      <c r="C13" t="n">
+        <v>6.466713666915894</v>
+      </c>
+      <c r="D13" t="n">
+        <v>5.453125</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>6.93</v>
+      </c>
+      <c r="B14" t="n">
+        <v>0.04000000000000001</v>
+      </c>
+      <c r="C14" t="n">
+        <v>5.264625072479248</v>
+      </c>
+      <c r="D14" t="n">
+        <v>3.765625</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>12.09</v>
+      </c>
+      <c r="B15" t="n">
+        <v>0.36</v>
+      </c>
+      <c r="C15" t="n">
+        <v>36.54512047767639</v>
+      </c>
+      <c r="D15" t="n">
+        <v>35.78125</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>8.49</v>
+      </c>
+      <c r="B16" t="n">
+        <v>1</v>
+      </c>
+      <c r="C16" t="n">
+        <v>85.68369960784912</v>
+      </c>
+      <c r="D16" t="n">
+        <v>76.90625</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>11.92</v>
+      </c>
+      <c r="B17" t="n">
+        <v>1</v>
+      </c>
+      <c r="C17" t="n">
+        <v>55.40087199211121</v>
+      </c>
+      <c r="D17" t="n">
+        <v>52.15625</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>16.63</v>
+      </c>
+      <c r="B18" t="n">
+        <v>1</v>
+      </c>
+      <c r="C18" t="n">
+        <v>47.94355058670044</v>
+      </c>
+      <c r="D18" t="n">
+        <v>44.859375</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>37.37</v>
+      </c>
+      <c r="B19" t="n">
+        <v>0.36</v>
+      </c>
+      <c r="C19" t="n">
+        <v>22.59253191947937</v>
+      </c>
+      <c r="D19" t="n">
+        <v>21.375</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>39.78</v>
+      </c>
+      <c r="B20" t="n">
+        <v>0.16</v>
+      </c>
+      <c r="C20" t="n">
+        <v>10.75686597824097</v>
+      </c>
+      <c r="D20" t="n">
+        <v>10.21875</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>37.37</v>
+      </c>
+      <c r="B21" t="n">
+        <v>0.36</v>
+      </c>
+      <c r="C21" t="n">
+        <v>21.32076287269592</v>
+      </c>
+      <c r="D21" t="n">
+        <v>20.75</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>37.37</v>
+      </c>
+      <c r="B22" t="n">
+        <v>0.36</v>
+      </c>
+      <c r="C22" t="n">
+        <v>21.63731241226196</v>
+      </c>
+      <c r="D22" t="n">
+        <v>21.046875</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>17.84</v>
+      </c>
+      <c r="B23" t="n">
+        <v>0.36</v>
+      </c>
+      <c r="C23" t="n">
+        <v>17.41600775718689</v>
+      </c>
+      <c r="D23" t="n">
+        <v>15.5625</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>17.84</v>
+      </c>
+      <c r="B24" t="n">
+        <v>0.36</v>
+      </c>
+      <c r="C24" t="n">
+        <v>18.63977336883545</v>
+      </c>
+      <c r="D24" t="n">
+        <v>17.265625</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>17.84</v>
+      </c>
+      <c r="B25" t="n">
+        <v>0.36</v>
+      </c>
+      <c r="C25" t="n">
+        <v>15.21477603912354</v>
+      </c>
+      <c r="D25" t="n">
+        <v>14.625</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>17.84</v>
+      </c>
+      <c r="B26" t="n">
+        <v>0.36</v>
+      </c>
+      <c r="C26" t="n">
+        <v>15.69570708274841</v>
+      </c>
+      <c r="D26" t="n">
+        <v>14.671875</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>17.84</v>
+      </c>
+      <c r="B27" t="n">
+        <v>0.36</v>
+      </c>
+      <c r="C27" t="n">
+        <v>21.96741771697998</v>
+      </c>
+      <c r="D27" t="n">
+        <v>20.890625</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>39.06</v>
+      </c>
+      <c r="B28" t="n">
+        <v>0.04000000000000001</v>
+      </c>
+      <c r="C28" t="n">
+        <v>2.837246417999268</v>
+      </c>
+      <c r="D28" t="n">
+        <v>2.34375</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>37.37</v>
+      </c>
+      <c r="B29" t="n">
+        <v>0.36</v>
+      </c>
+      <c r="C29" t="n">
+        <v>25.06726121902466</v>
+      </c>
+      <c r="D29" t="n">
+        <v>24.34375</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>39.78</v>
+      </c>
+      <c r="B30" t="n">
+        <v>0.16</v>
+      </c>
+      <c r="C30" t="n">
+        <v>10.740394115448</v>
+      </c>
+      <c r="D30" t="n">
+        <v>18.109375</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>39.78</v>
+      </c>
+      <c r="B31" t="n">
+        <v>0.16</v>
+      </c>
+      <c r="C31" t="n">
+        <v>10.9668345451355</v>
+      </c>
+      <c r="D31" t="n">
+        <v>17.703125</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>39.78</v>
+      </c>
+      <c r="B32" t="n">
+        <v>0.16</v>
+      </c>
+      <c r="C32" t="n">
+        <v>12.74186491966248</v>
+      </c>
+      <c r="D32" t="n">
+        <v>12.203125</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
fixed the double mistake in get_white_black
</commit_message>
<xml_diff>
--- a/Modules/Main/results.xlsx
+++ b/Modules/Main/results.xlsx
@@ -424,7 +424,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D35"/>
+  <dimension ref="A1:D44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -915,6 +915,132 @@
         <v>5.984375</v>
       </c>
     </row>
+    <row r="36">
+      <c r="A36" t="n">
+        <v>17.84</v>
+      </c>
+      <c r="B36" t="n">
+        <v>0.36</v>
+      </c>
+      <c r="C36" t="n">
+        <v>20.19210028648376</v>
+      </c>
+      <c r="D36" t="n">
+        <v>6.46875</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="n">
+        <v>17.84</v>
+      </c>
+      <c r="B37" t="n">
+        <v>0.36</v>
+      </c>
+      <c r="C37" t="n">
+        <v>19.50743865966797</v>
+      </c>
+      <c r="D37" t="n">
+        <v>6.84375</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="n">
+        <v>17.84</v>
+      </c>
+      <c r="B38" t="n">
+        <v>0.36</v>
+      </c>
+      <c r="C38" t="n">
+        <v>18.69954299926758</v>
+      </c>
+      <c r="D38" t="n">
+        <v>6.921875</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="n">
+        <v>17.84</v>
+      </c>
+      <c r="B39" t="n">
+        <v>0.36</v>
+      </c>
+      <c r="C39" t="n">
+        <v>13.4420440196991</v>
+      </c>
+      <c r="D39" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="n">
+        <v>17.84</v>
+      </c>
+      <c r="B40" t="n">
+        <v>0.36</v>
+      </c>
+      <c r="C40" t="n">
+        <v>13.99964332580566</v>
+      </c>
+      <c r="D40" t="n">
+        <v>10.203125</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="n">
+        <v>37.37</v>
+      </c>
+      <c r="B41" t="n">
+        <v>0.36</v>
+      </c>
+      <c r="C41" t="n">
+        <v>18.73186135292053</v>
+      </c>
+      <c r="D41" t="n">
+        <v>15.734375</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="n">
+        <v>39.78</v>
+      </c>
+      <c r="B42" t="n">
+        <v>0.16</v>
+      </c>
+      <c r="C42" t="n">
+        <v>9.278669595718384</v>
+      </c>
+      <c r="D42" t="n">
+        <v>6.703125</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="n">
+        <v>39.78</v>
+      </c>
+      <c r="B43" t="n">
+        <v>0.16</v>
+      </c>
+      <c r="C43" t="n">
+        <v>8.955015659332275</v>
+      </c>
+      <c r="D43" t="n">
+        <v>7.125</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="n">
+        <v>39.78</v>
+      </c>
+      <c r="B44" t="n">
+        <v>0.16</v>
+      </c>
+      <c r="C44" t="n">
+        <v>8.963810920715332</v>
+      </c>
+      <c r="D44" t="n">
+        <v>6.8125</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added the code variables, above line distances
</commit_message>
<xml_diff>
--- a/Modules/Main/results.xlsx
+++ b/Modules/Main/results.xlsx
@@ -424,7 +424,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -471,6 +471,193 @@
         <v>2.833401441574097</v>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>39.06</v>
+      </c>
+      <c r="B4" t="n">
+        <v>0.04000000000000001</v>
+      </c>
+      <c r="C4" t="n">
+        <v>3.029262542724609</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>39.06</v>
+      </c>
+      <c r="B5" t="n">
+        <v>0.04000000000000001</v>
+      </c>
+      <c r="C5" t="n">
+        <v>3.055202484130859</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>39.06</v>
+      </c>
+      <c r="B6" t="n">
+        <v>0.04000000000000001</v>
+      </c>
+      <c r="C6" t="n">
+        <v>3.826434135437012</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>37.37</v>
+      </c>
+      <c r="B7" t="n">
+        <v>0.36</v>
+      </c>
+      <c r="C7" t="n">
+        <v>22.244460105896</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>39.06</v>
+      </c>
+      <c r="B8" t="n">
+        <v>0.04000000000000001</v>
+      </c>
+      <c r="C8" t="n">
+        <v>3.323311328887939</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>37.37</v>
+      </c>
+      <c r="B9" t="n">
+        <v>0.36</v>
+      </c>
+      <c r="C9" t="n">
+        <v>20.74647331237793</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>39.06</v>
+      </c>
+      <c r="B10" t="n">
+        <v>0.04000000000000001</v>
+      </c>
+      <c r="C10" t="n">
+        <v>2.801284313201904</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>37.37</v>
+      </c>
+      <c r="B11" t="n">
+        <v>0.36</v>
+      </c>
+      <c r="C11" t="n">
+        <v>20.7770311832428</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>39.06</v>
+      </c>
+      <c r="B12" t="n">
+        <v>0.04000000000000001</v>
+      </c>
+      <c r="C12" t="n">
+        <v>3.219979524612427</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>37.37</v>
+      </c>
+      <c r="B13" t="n">
+        <v>0.36</v>
+      </c>
+      <c r="C13" t="n">
+        <v>20.27344155311584</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>39.06</v>
+      </c>
+      <c r="B14" t="n">
+        <v>0.04000000000000001</v>
+      </c>
+      <c r="C14" t="n">
+        <v>2.994482517242432</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>39.06</v>
+      </c>
+      <c r="B15" t="n">
+        <v>0.04000000000000001</v>
+      </c>
+      <c r="C15" t="n">
+        <v>2.753181219100952</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>39.06</v>
+      </c>
+      <c r="B16" t="n">
+        <v>0.04000000000000001</v>
+      </c>
+      <c r="C16" t="n">
+        <v>2.686118364334106</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>37.37</v>
+      </c>
+      <c r="B17" t="n">
+        <v>0.36</v>
+      </c>
+      <c r="C17" t="n">
+        <v>20.11983466148376</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>39.06</v>
+      </c>
+      <c r="B18" t="n">
+        <v>0.04000000000000001</v>
+      </c>
+      <c r="C18" t="n">
+        <v>3.07470440864563</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>39.06</v>
+      </c>
+      <c r="B19" t="n">
+        <v>0.04000000000000001</v>
+      </c>
+      <c r="C19" t="n">
+        <v>3.950433254241943</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>39.06</v>
+      </c>
+      <c r="B20" t="n">
+        <v>0.04000000000000001</v>
+      </c>
+      <c r="C20" t="n">
+        <v>3.116287708282471</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
acyah fix distance and part of inboxes
</commit_message>
<xml_diff>
--- a/Modules/Main/results.xlsx
+++ b/Modules/Main/results.xlsx
@@ -424,7 +424,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D82"/>
+  <dimension ref="A1:D107"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -1573,6 +1573,356 @@
         <v>9.375</v>
       </c>
     </row>
+    <row r="83">
+      <c r="A83" t="n">
+        <v>39.78</v>
+      </c>
+      <c r="B83" t="n">
+        <v>0.16</v>
+      </c>
+      <c r="C83" t="n">
+        <v>13.04704260826111</v>
+      </c>
+      <c r="D83" t="n">
+        <v>12.671875</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="n">
+        <v>39.78</v>
+      </c>
+      <c r="B84" t="n">
+        <v>0.16</v>
+      </c>
+      <c r="C84" t="n">
+        <v>17.27826714515686</v>
+      </c>
+      <c r="D84" t="n">
+        <v>15.03125</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="n">
+        <v>20.38</v>
+      </c>
+      <c r="B85" t="n">
+        <v>0.16</v>
+      </c>
+      <c r="C85" t="n">
+        <v>11.11862778663635</v>
+      </c>
+      <c r="D85" t="n">
+        <v>9.453125</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="n">
+        <v>26.1</v>
+      </c>
+      <c r="B86" t="n">
+        <v>0.16</v>
+      </c>
+      <c r="C86" t="n">
+        <v>12.31966423988342</v>
+      </c>
+      <c r="D86" t="n">
+        <v>10.71875</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="n">
+        <v>24.85</v>
+      </c>
+      <c r="B87" t="n">
+        <v>0.36</v>
+      </c>
+      <c r="C87" t="n">
+        <v>23.62781620025635</v>
+      </c>
+      <c r="D87" t="n">
+        <v>22.515625</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="n">
+        <v>39.06</v>
+      </c>
+      <c r="B88" t="n">
+        <v>0.04000000000000001</v>
+      </c>
+      <c r="C88" t="n">
+        <v>14.29457950592041</v>
+      </c>
+      <c r="D88" t="n">
+        <v>12.515625</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="n">
+        <v>37.37</v>
+      </c>
+      <c r="B89" t="n">
+        <v>0.36</v>
+      </c>
+      <c r="C89" t="n">
+        <v>36.94248414039612</v>
+      </c>
+      <c r="D89" t="n">
+        <v>35.90625</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="n">
+        <v>29.36</v>
+      </c>
+      <c r="B90" t="n">
+        <v>0.04000000000000001</v>
+      </c>
+      <c r="C90" t="n">
+        <v>3.250525951385498</v>
+      </c>
+      <c r="D90" t="n">
+        <v>2.125</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="n">
+        <v>24.16</v>
+      </c>
+      <c r="B91" t="n">
+        <v>0.36</v>
+      </c>
+      <c r="C91" t="n">
+        <v>18.95114183425903</v>
+      </c>
+      <c r="D91" t="n">
+        <v>16.75</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="n">
+        <v>46.83</v>
+      </c>
+      <c r="B92" t="n">
+        <v>0.36</v>
+      </c>
+      <c r="C92" t="n">
+        <v>23.58631563186646</v>
+      </c>
+      <c r="D92" t="n">
+        <v>21.640625</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="n">
+        <v>96.31999999999999</v>
+      </c>
+      <c r="B93" t="n">
+        <v>0.36</v>
+      </c>
+      <c r="C93" t="n">
+        <v>40.86225938796997</v>
+      </c>
+      <c r="D93" t="n">
+        <v>38.46875</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="n">
+        <v>94.73999999999999</v>
+      </c>
+      <c r="B94" t="n">
+        <v>0.04000000000000001</v>
+      </c>
+      <c r="C94" t="n">
+        <v>5.92878532409668</v>
+      </c>
+      <c r="D94" t="n">
+        <v>5.3125</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="n">
+        <v>96.31999999999999</v>
+      </c>
+      <c r="B95" t="n">
+        <v>0.36</v>
+      </c>
+      <c r="C95" t="n">
+        <v>47.24303102493286</v>
+      </c>
+      <c r="D95" t="n">
+        <v>45.703125</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="n">
+        <v>59.03</v>
+      </c>
+      <c r="B96" t="n">
+        <v>0.36</v>
+      </c>
+      <c r="C96" t="n">
+        <v>44.20377826690674</v>
+      </c>
+      <c r="D96" t="n">
+        <v>41.921875</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="n">
+        <v>93.62</v>
+      </c>
+      <c r="B97" t="n">
+        <v>0.16</v>
+      </c>
+      <c r="C97" t="n">
+        <v>20.47512221336365</v>
+      </c>
+      <c r="D97" t="n">
+        <v>19.171875</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="n">
+        <v>93.62</v>
+      </c>
+      <c r="B98" t="n">
+        <v>0.16</v>
+      </c>
+      <c r="C98" t="n">
+        <v>30.63012337684631</v>
+      </c>
+      <c r="D98" t="n">
+        <v>28.515625</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="n">
+        <v>96.31999999999999</v>
+      </c>
+      <c r="B99" t="n">
+        <v>0.36</v>
+      </c>
+      <c r="C99" t="n">
+        <v>81.34160351753235</v>
+      </c>
+      <c r="D99" t="n">
+        <v>79.765625</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="n">
+        <v>93.62</v>
+      </c>
+      <c r="B100" t="n">
+        <v>0.16</v>
+      </c>
+      <c r="C100" t="n">
+        <v>20.86597800254822</v>
+      </c>
+      <c r="D100" t="n">
+        <v>19.8125</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="n">
+        <v>39.78</v>
+      </c>
+      <c r="B101" t="n">
+        <v>0.16</v>
+      </c>
+      <c r="C101" t="n">
+        <v>22.68091750144958</v>
+      </c>
+      <c r="D101" t="n">
+        <v>21.125</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="n">
+        <v>39.78</v>
+      </c>
+      <c r="B102" t="n">
+        <v>0.16</v>
+      </c>
+      <c r="C102" t="n">
+        <v>43.15804982185364</v>
+      </c>
+      <c r="D102" t="n">
+        <v>38.28125</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="n">
+        <v>60.22</v>
+      </c>
+      <c r="B103" t="n">
+        <v>0.16</v>
+      </c>
+      <c r="C103" t="n">
+        <v>43.08988738059998</v>
+      </c>
+      <c r="D103" t="n">
+        <v>41.640625</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="n">
+        <v>39.78</v>
+      </c>
+      <c r="B104" t="n">
+        <v>0.16</v>
+      </c>
+      <c r="C104" t="n">
+        <v>14.59283208847046</v>
+      </c>
+      <c r="D104" t="n">
+        <v>14.484375</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="n">
+        <v>39.78</v>
+      </c>
+      <c r="B105" t="n">
+        <v>0.16</v>
+      </c>
+      <c r="C105" t="n">
+        <v>25.07989716529846</v>
+      </c>
+      <c r="D105" t="n">
+        <v>23.78125</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="n">
+        <v>39.78</v>
+      </c>
+      <c r="B106" t="n">
+        <v>0.16</v>
+      </c>
+      <c r="C106" t="n">
+        <v>29.23488664627075</v>
+      </c>
+      <c r="D106" t="n">
+        <v>24.59375</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="n">
+        <v>39.78</v>
+      </c>
+      <c r="B107" t="n">
+        <v>0.16</v>
+      </c>
+      <c r="C107" t="n">
+        <v>20.58482432365417</v>
+      </c>
+      <c r="D107" t="n">
+        <v>18.8125</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
fixed the dictionary bag
</commit_message>
<xml_diff>
--- a/Modules/Main/results.xlsx
+++ b/Modules/Main/results.xlsx
@@ -424,7 +424,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D107"/>
+  <dimension ref="A1:D111"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -1923,6 +1923,62 @@
         <v>18.8125</v>
       </c>
     </row>
+    <row r="108">
+      <c r="A108" t="n">
+        <v>39.78</v>
+      </c>
+      <c r="B108" t="n">
+        <v>0.16</v>
+      </c>
+      <c r="C108" t="n">
+        <v>10.01247477531433</v>
+      </c>
+      <c r="D108" t="n">
+        <v>9.3125</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="n">
+        <v>39.78</v>
+      </c>
+      <c r="B109" t="n">
+        <v>0.16</v>
+      </c>
+      <c r="C109" t="n">
+        <v>9.666251182556152</v>
+      </c>
+      <c r="D109" t="n">
+        <v>9.03125</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="n">
+        <v>39.78</v>
+      </c>
+      <c r="B110" t="n">
+        <v>0.16</v>
+      </c>
+      <c r="C110" t="n">
+        <v>9.286051273345947</v>
+      </c>
+      <c r="D110" t="n">
+        <v>8.796875</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="n">
+        <v>39.78</v>
+      </c>
+      <c r="B111" t="n">
+        <v>0.16</v>
+      </c>
+      <c r="C111" t="n">
+        <v>9.419345617294312</v>
+      </c>
+      <c r="D111" t="n">
+        <v>8.84375</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added building to main module
</commit_message>
<xml_diff>
--- a/Modules/Main/results.xlsx
+++ b/Modules/Main/results.xlsx
@@ -424,7 +424,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D90"/>
+  <dimension ref="A1:D95"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -1685,6 +1685,76 @@
         <v>9.234375</v>
       </c>
     </row>
+    <row r="91">
+      <c r="A91" t="n">
+        <v>39.78</v>
+      </c>
+      <c r="B91" t="n">
+        <v>0.16</v>
+      </c>
+      <c r="C91" t="n">
+        <v>70.68860268592834</v>
+      </c>
+      <c r="D91" t="n">
+        <v>138.890625</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="n">
+        <v>39.78</v>
+      </c>
+      <c r="B92" t="n">
+        <v>0.16</v>
+      </c>
+      <c r="C92" t="n">
+        <v>245.2299783229828</v>
+      </c>
+      <c r="D92" t="n">
+        <v>149.359375</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="n">
+        <v>39.78</v>
+      </c>
+      <c r="B93" t="n">
+        <v>0.16</v>
+      </c>
+      <c r="C93" t="n">
+        <v>74.51772165298462</v>
+      </c>
+      <c r="D93" t="n">
+        <v>128.265625</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="n">
+        <v>39.78</v>
+      </c>
+      <c r="B94" t="n">
+        <v>0.16</v>
+      </c>
+      <c r="C94" t="n">
+        <v>79.88404107093811</v>
+      </c>
+      <c r="D94" t="n">
+        <v>137.375</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="n">
+        <v>39.78</v>
+      </c>
+      <c r="B95" t="n">
+        <v>0.16</v>
+      </c>
+      <c r="C95" t="n">
+        <v>73.88481378555298</v>
+      </c>
+      <c r="D95" t="n">
+        <v>120.9375</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added structures to full detection
</commit_message>
<xml_diff>
--- a/Modules/Main/results.xlsx
+++ b/Modules/Main/results.xlsx
@@ -424,7 +424,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D95"/>
+  <dimension ref="A1:D105"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -1755,6 +1755,146 @@
         <v>120.9375</v>
       </c>
     </row>
+    <row r="96">
+      <c r="A96" t="n">
+        <v>39.78</v>
+      </c>
+      <c r="B96" t="n">
+        <v>0.16</v>
+      </c>
+      <c r="C96" t="n">
+        <v>67.54763293266296</v>
+      </c>
+      <c r="D96" t="n">
+        <v>114.03125</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="n">
+        <v>39.78</v>
+      </c>
+      <c r="B97" t="n">
+        <v>0.16</v>
+      </c>
+      <c r="C97" t="n">
+        <v>71.40265464782715</v>
+      </c>
+      <c r="D97" t="n">
+        <v>125.984375</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="n">
+        <v>39.78</v>
+      </c>
+      <c r="B98" t="n">
+        <v>0.16</v>
+      </c>
+      <c r="C98" t="n">
+        <v>63.66919302940369</v>
+      </c>
+      <c r="D98" t="n">
+        <v>110.875</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="n">
+        <v>39.78</v>
+      </c>
+      <c r="B99" t="n">
+        <v>0.16</v>
+      </c>
+      <c r="C99" t="n">
+        <v>74.6501157283783</v>
+      </c>
+      <c r="D99" t="n">
+        <v>126.1875</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="n">
+        <v>50.43</v>
+      </c>
+      <c r="B100" t="n">
+        <v>0.16</v>
+      </c>
+      <c r="C100" t="n">
+        <v>80.41346979141235</v>
+      </c>
+      <c r="D100" t="n">
+        <v>127.59375</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="n">
+        <v>50.43</v>
+      </c>
+      <c r="B101" t="n">
+        <v>0.16</v>
+      </c>
+      <c r="C101" t="n">
+        <v>86.68496823310852</v>
+      </c>
+      <c r="D101" t="n">
+        <v>144.9375</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="n">
+        <v>99.67</v>
+      </c>
+      <c r="B102" t="n">
+        <v>0.16</v>
+      </c>
+      <c r="C102" t="n">
+        <v>85.03541254997253</v>
+      </c>
+      <c r="D102" t="n">
+        <v>141.15625</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="n">
+        <v>10.65</v>
+      </c>
+      <c r="B103" t="n">
+        <v>0.16</v>
+      </c>
+      <c r="C103" t="n">
+        <v>67.56848335266113</v>
+      </c>
+      <c r="D103" t="n">
+        <v>118.265625</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="n">
+        <v>39.78</v>
+      </c>
+      <c r="B104" t="n">
+        <v>0.16</v>
+      </c>
+      <c r="C104" t="n">
+        <v>63.21611595153809</v>
+      </c>
+      <c r="D104" t="n">
+        <v>100.875</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="n">
+        <v>20.78</v>
+      </c>
+      <c r="B105" t="n">
+        <v>0.16</v>
+      </c>
+      <c r="C105" t="n">
+        <v>66.74141430854797</v>
+      </c>
+      <c r="D105" t="n">
+        <v>113.921875</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
fix bug and move building to comment for tomorrow
</commit_message>
<xml_diff>
--- a/Modules/Main/results.xlsx
+++ b/Modules/Main/results.xlsx
@@ -424,7 +424,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D111"/>
+  <dimension ref="A1:D119"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -1581,10 +1581,10 @@
         <v>0.16</v>
       </c>
       <c r="C83" t="n">
-        <v>16.95105242729187</v>
+        <v>13.04704260826111</v>
       </c>
       <c r="D83" t="n">
-        <v>8.8125</v>
+        <v>12.671875</v>
       </c>
     </row>
     <row r="84">
@@ -1595,276 +1595,276 @@
         <v>0.16</v>
       </c>
       <c r="C84" t="n">
-        <v>15.44545221328735</v>
+        <v>17.27826714515686</v>
       </c>
       <c r="D84" t="n">
-        <v>10.046875</v>
+        <v>15.03125</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="n">
-        <v>39.78</v>
+        <v>20.38</v>
       </c>
       <c r="B85" t="n">
         <v>0.16</v>
       </c>
       <c r="C85" t="n">
-        <v>16.70379161834717</v>
+        <v>11.11862778663635</v>
       </c>
       <c r="D85" t="n">
-        <v>10.875</v>
+        <v>9.453125</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="n">
-        <v>39.78</v>
+        <v>26.1</v>
       </c>
       <c r="B86" t="n">
         <v>0.16</v>
       </c>
       <c r="C86" t="n">
-        <v>15.54907369613647</v>
+        <v>12.31966423988342</v>
       </c>
       <c r="D86" t="n">
-        <v>8.46875</v>
+        <v>10.71875</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="n">
-        <v>39.78</v>
+        <v>24.85</v>
       </c>
       <c r="B87" t="n">
-        <v>0.16</v>
+        <v>0.36</v>
       </c>
       <c r="C87" t="n">
-        <v>15.18528008460999</v>
+        <v>23.62781620025635</v>
       </c>
       <c r="D87" t="n">
-        <v>8.5625</v>
+        <v>22.515625</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="n">
-        <v>39.78</v>
+        <v>39.06</v>
       </c>
       <c r="B88" t="n">
-        <v>0.16</v>
+        <v>0.04000000000000001</v>
       </c>
       <c r="C88" t="n">
-        <v>14.61031484603882</v>
+        <v>14.29457950592041</v>
       </c>
       <c r="D88" t="n">
-        <v>8.015625</v>
+        <v>12.515625</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="n">
-        <v>39.78</v>
+        <v>37.37</v>
       </c>
       <c r="B89" t="n">
-        <v>0.16</v>
+        <v>0.36</v>
       </c>
       <c r="C89" t="n">
-        <v>14.58043742179871</v>
+        <v>36.94248414039612</v>
       </c>
       <c r="D89" t="n">
-        <v>8.875</v>
+        <v>35.90625</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="n">
-        <v>39.78</v>
+        <v>29.36</v>
       </c>
       <c r="B90" t="n">
-        <v>0.16</v>
+        <v>0.04000000000000001</v>
       </c>
       <c r="C90" t="n">
-        <v>15.43518376350403</v>
+        <v>3.250525951385498</v>
       </c>
       <c r="D90" t="n">
-        <v>9.234375</v>
+        <v>2.125</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="n">
-        <v>39.78</v>
+        <v>24.16</v>
       </c>
       <c r="B91" t="n">
-        <v>0.16</v>
+        <v>0.36</v>
       </c>
       <c r="C91" t="n">
-        <v>70.68860268592834</v>
+        <v>18.95114183425903</v>
       </c>
       <c r="D91" t="n">
-        <v>138.890625</v>
+        <v>16.75</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="n">
-        <v>39.78</v>
+        <v>46.83</v>
       </c>
       <c r="B92" t="n">
-        <v>0.16</v>
+        <v>0.36</v>
       </c>
       <c r="C92" t="n">
-        <v>245.2299783229828</v>
+        <v>23.58631563186646</v>
       </c>
       <c r="D92" t="n">
-        <v>149.359375</v>
+        <v>21.640625</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="n">
-        <v>39.78</v>
+        <v>96.31999999999999</v>
       </c>
       <c r="B93" t="n">
-        <v>0.16</v>
+        <v>0.36</v>
       </c>
       <c r="C93" t="n">
-        <v>74.51772165298462</v>
+        <v>40.86225938796997</v>
       </c>
       <c r="D93" t="n">
-        <v>128.265625</v>
+        <v>38.46875</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="n">
-        <v>39.78</v>
+        <v>94.73999999999999</v>
       </c>
       <c r="B94" t="n">
-        <v>0.16</v>
+        <v>0.04000000000000001</v>
       </c>
       <c r="C94" t="n">
-        <v>79.88404107093811</v>
+        <v>5.92878532409668</v>
       </c>
       <c r="D94" t="n">
-        <v>137.375</v>
+        <v>5.3125</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="n">
-        <v>39.78</v>
+        <v>96.31999999999999</v>
       </c>
       <c r="B95" t="n">
-        <v>0.16</v>
+        <v>0.36</v>
       </c>
       <c r="C95" t="n">
-        <v>73.88481378555298</v>
+        <v>47.24303102493286</v>
       </c>
       <c r="D95" t="n">
-        <v>120.9375</v>
+        <v>45.703125</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="n">
-        <v>39.78</v>
+        <v>59.03</v>
       </c>
       <c r="B96" t="n">
-        <v>0.16</v>
+        <v>0.36</v>
       </c>
       <c r="C96" t="n">
-        <v>67.54763293266296</v>
+        <v>44.20377826690674</v>
       </c>
       <c r="D96" t="n">
-        <v>114.03125</v>
+        <v>41.921875</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="n">
-        <v>39.78</v>
+        <v>93.62</v>
       </c>
       <c r="B97" t="n">
         <v>0.16</v>
       </c>
       <c r="C97" t="n">
-        <v>71.40265464782715</v>
+        <v>20.47512221336365</v>
       </c>
       <c r="D97" t="n">
-        <v>125.984375</v>
+        <v>19.171875</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="n">
-        <v>39.78</v>
+        <v>93.62</v>
       </c>
       <c r="B98" t="n">
         <v>0.16</v>
       </c>
       <c r="C98" t="n">
-        <v>63.66919302940369</v>
+        <v>30.63012337684631</v>
       </c>
       <c r="D98" t="n">
-        <v>110.875</v>
+        <v>28.515625</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="n">
-        <v>39.78</v>
+        <v>96.31999999999999</v>
       </c>
       <c r="B99" t="n">
-        <v>0.16</v>
+        <v>0.36</v>
       </c>
       <c r="C99" t="n">
-        <v>74.6501157283783</v>
+        <v>81.34160351753235</v>
       </c>
       <c r="D99" t="n">
-        <v>126.1875</v>
+        <v>79.765625</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="n">
-        <v>50.43</v>
+        <v>93.62</v>
       </c>
       <c r="B100" t="n">
         <v>0.16</v>
       </c>
       <c r="C100" t="n">
-        <v>80.41346979141235</v>
+        <v>20.86597800254822</v>
       </c>
       <c r="D100" t="n">
-        <v>127.59375</v>
+        <v>19.8125</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="n">
-        <v>50.43</v>
+        <v>39.78</v>
       </c>
       <c r="B101" t="n">
         <v>0.16</v>
       </c>
       <c r="C101" t="n">
-        <v>86.68496823310852</v>
+        <v>22.68091750144958</v>
       </c>
       <c r="D101" t="n">
-        <v>144.9375</v>
+        <v>21.125</v>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="n">
-        <v>99.67</v>
+        <v>39.78</v>
       </c>
       <c r="B102" t="n">
         <v>0.16</v>
       </c>
       <c r="C102" t="n">
-        <v>85.03541254997253</v>
+        <v>43.15804982185364</v>
       </c>
       <c r="D102" t="n">
-        <v>141.15625</v>
+        <v>38.28125</v>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="n">
-        <v>10.65</v>
+        <v>60.22</v>
       </c>
       <c r="B103" t="n">
         <v>0.16</v>
       </c>
       <c r="C103" t="n">
-        <v>67.56848335266113</v>
+        <v>43.08988738059998</v>
       </c>
       <c r="D103" t="n">
-        <v>118.265625</v>
+        <v>41.640625</v>
       </c>
     </row>
     <row r="104">
@@ -1875,108 +1875,220 @@
         <v>0.16</v>
       </c>
       <c r="C104" t="n">
-        <v>63.21611595153809</v>
+        <v>14.59283208847046</v>
       </c>
       <c r="D104" t="n">
-        <v>100.875</v>
+        <v>14.484375</v>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="n">
-        <v>20.78</v>
+        <v>39.78</v>
       </c>
       <c r="B105" t="n">
         <v>0.16</v>
       </c>
       <c r="C105" t="n">
-        <v>66.74141430854797</v>
+        <v>25.07989716529846</v>
       </c>
       <c r="D105" t="n">
-        <v>113.921875</v>
+        <v>23.78125</v>
       </c>
     </row>
     <row r="106">
       <c r="A106" t="n">
-        <v>98.62</v>
+        <v>39.78</v>
       </c>
       <c r="B106" t="n">
         <v>0.16</v>
       </c>
       <c r="C106" t="n">
-        <v>85.15410208702087</v>
+        <v>29.23488664627075</v>
       </c>
       <c r="D106" t="n">
-        <v>136.90625</v>
+        <v>24.59375</v>
       </c>
     </row>
     <row r="107">
       <c r="A107" t="n">
-        <v>100</v>
+        <v>39.78</v>
       </c>
       <c r="B107" t="n">
         <v>0.16</v>
       </c>
       <c r="C107" t="n">
-        <v>84.77142000198364</v>
+        <v>20.58482432365417</v>
       </c>
       <c r="D107" t="n">
-        <v>124.875</v>
+        <v>18.8125</v>
       </c>
     </row>
     <row r="108">
       <c r="A108" t="n">
-        <v>99.87</v>
+        <v>39.78</v>
       </c>
       <c r="B108" t="n">
         <v>0.16</v>
       </c>
       <c r="C108" t="n">
-        <v>84.77447628974915</v>
+        <v>20.68654370307922</v>
       </c>
       <c r="D108" t="n">
-        <v>132.125</v>
+        <v>17.3125</v>
       </c>
     </row>
     <row r="109">
       <c r="A109" t="n">
-        <v>95.59999999999999</v>
+        <v>39.78</v>
       </c>
       <c r="B109" t="n">
         <v>0.16</v>
       </c>
       <c r="C109" t="n">
-        <v>76.76323866844177</v>
+        <v>17.747483253479</v>
       </c>
       <c r="D109" t="n">
-        <v>129.484375</v>
+        <v>15.734375</v>
       </c>
     </row>
     <row r="110">
       <c r="A110" t="n">
-        <v>96.58</v>
+        <v>39.78</v>
       </c>
       <c r="B110" t="n">
         <v>0.16</v>
       </c>
       <c r="C110" t="n">
-        <v>80.26044988632202</v>
+        <v>13.60085797309875</v>
       </c>
       <c r="D110" t="n">
-        <v>133.78125</v>
+        <v>12.625</v>
       </c>
     </row>
     <row r="111">
       <c r="A111" t="n">
-        <v>98.65000000000001</v>
+        <v>39.78</v>
       </c>
       <c r="B111" t="n">
-        <v>1</v>
+        <v>0.16</v>
       </c>
       <c r="C111" t="n">
-        <v>431.6280508041382</v>
+        <v>14.34477090835571</v>
       </c>
       <c r="D111" t="n">
-        <v>606.125</v>
+        <v>15.125</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="n">
+        <v>39.78</v>
+      </c>
+      <c r="B112" t="n">
+        <v>0.16</v>
+      </c>
+      <c r="C112" t="n">
+        <v>14.43962907791138</v>
+      </c>
+      <c r="D112" t="n">
+        <v>13.84375</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="n">
+        <v>20.38</v>
+      </c>
+      <c r="B113" t="n">
+        <v>0.16</v>
+      </c>
+      <c r="C113" t="n">
+        <v>17.18347358703613</v>
+      </c>
+      <c r="D113" t="n">
+        <v>17.40625</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="n">
+        <v>39.78</v>
+      </c>
+      <c r="B114" t="n">
+        <v>0.16</v>
+      </c>
+      <c r="C114" t="n">
+        <v>20.92087531089783</v>
+      </c>
+      <c r="D114" t="n">
+        <v>20.125</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="n">
+        <v>39.78</v>
+      </c>
+      <c r="B115" t="n">
+        <v>0.16</v>
+      </c>
+      <c r="C115" t="n">
+        <v>24.21634316444397</v>
+      </c>
+      <c r="D115" t="n">
+        <v>23.03125</v>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="n">
+        <v>39.06</v>
+      </c>
+      <c r="B116" t="n">
+        <v>0.04000000000000001</v>
+      </c>
+      <c r="C116" t="n">
+        <v>10.04663562774658</v>
+      </c>
+      <c r="D116" t="n">
+        <v>9.296875</v>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="n">
+        <v>39.78</v>
+      </c>
+      <c r="B117" t="n">
+        <v>0.16</v>
+      </c>
+      <c r="C117" t="n">
+        <v>24.07325077056885</v>
+      </c>
+      <c r="D117" t="n">
+        <v>23.078125</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="n">
+        <v>39.78</v>
+      </c>
+      <c r="B118" t="n">
+        <v>0.16</v>
+      </c>
+      <c r="C118" t="n">
+        <v>20.16321396827698</v>
+      </c>
+      <c r="D118" t="n">
+        <v>18.1875</v>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="n">
+        <v>39.78</v>
+      </c>
+      <c r="B119" t="n">
+        <v>0.16</v>
+      </c>
+      <c r="C119" t="n">
+        <v>17.94358134269714</v>
+      </c>
+      <c r="D119" t="n">
+        <v>17.03125</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
improve gui for buildings to
</commit_message>
<xml_diff>
--- a/Modules/Main/results.xlsx
+++ b/Modules/Main/results.xlsx
@@ -424,7 +424,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D165"/>
+  <dimension ref="A1:D178"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -2735,6 +2735,188 @@
         <v>20.671875</v>
       </c>
     </row>
+    <row r="166">
+      <c r="A166" t="n">
+        <v>84.2</v>
+      </c>
+      <c r="B166" t="n">
+        <v>0.36</v>
+      </c>
+      <c r="C166" t="n">
+        <v>118.7564432621002</v>
+      </c>
+      <c r="D166" t="n">
+        <v>111.640625</v>
+      </c>
+    </row>
+    <row r="167">
+      <c r="A167" t="n">
+        <v>84.2</v>
+      </c>
+      <c r="B167" t="n">
+        <v>0.36</v>
+      </c>
+      <c r="C167" t="n">
+        <v>180.320063829422</v>
+      </c>
+      <c r="D167" t="n">
+        <v>178.1875</v>
+      </c>
+    </row>
+    <row r="168">
+      <c r="A168" t="n">
+        <v>39.78</v>
+      </c>
+      <c r="B168" t="n">
+        <v>0.16</v>
+      </c>
+      <c r="C168" t="n">
+        <v>32.275066614151</v>
+      </c>
+      <c r="D168" t="n">
+        <v>30.96875</v>
+      </c>
+    </row>
+    <row r="169">
+      <c r="A169" t="n">
+        <v>39.78</v>
+      </c>
+      <c r="B169" t="n">
+        <v>0.16</v>
+      </c>
+      <c r="C169" t="n">
+        <v>67.87305283546448</v>
+      </c>
+      <c r="D169" t="n">
+        <v>49.28125</v>
+      </c>
+    </row>
+    <row r="170">
+      <c r="A170" t="n">
+        <v>39.78</v>
+      </c>
+      <c r="B170" t="n">
+        <v>0.16</v>
+      </c>
+      <c r="C170" t="n">
+        <v>29.76566123962402</v>
+      </c>
+      <c r="D170" t="n">
+        <v>28.8125</v>
+      </c>
+    </row>
+    <row r="171">
+      <c r="A171" t="n">
+        <v>39.78</v>
+      </c>
+      <c r="B171" t="n">
+        <v>0.16</v>
+      </c>
+      <c r="C171" t="n">
+        <v>29.20565843582153</v>
+      </c>
+      <c r="D171" t="n">
+        <v>28.984375</v>
+      </c>
+    </row>
+    <row r="172">
+      <c r="A172" t="n">
+        <v>39.78</v>
+      </c>
+      <c r="B172" t="n">
+        <v>0.16</v>
+      </c>
+      <c r="C172" t="n">
+        <v>19.59266972541809</v>
+      </c>
+      <c r="D172" t="n">
+        <v>19.453125</v>
+      </c>
+    </row>
+    <row r="173">
+      <c r="A173" t="n">
+        <v>39.78</v>
+      </c>
+      <c r="B173" t="n">
+        <v>0.16</v>
+      </c>
+      <c r="C173" t="n">
+        <v>39.31414198875427</v>
+      </c>
+      <c r="D173" t="n">
+        <v>39.421875</v>
+      </c>
+    </row>
+    <row r="174">
+      <c r="A174" t="n">
+        <v>39.06</v>
+      </c>
+      <c r="B174" t="n">
+        <v>0.04000000000000001</v>
+      </c>
+      <c r="C174" t="n">
+        <v>5.450976371765137</v>
+      </c>
+      <c r="D174" t="n">
+        <v>5.34375</v>
+      </c>
+    </row>
+    <row r="175">
+      <c r="A175" t="n">
+        <v>39.06</v>
+      </c>
+      <c r="B175" t="n">
+        <v>0.04000000000000001</v>
+      </c>
+      <c r="C175" t="n">
+        <v>7.199516773223877</v>
+      </c>
+      <c r="D175" t="n">
+        <v>7.1875</v>
+      </c>
+    </row>
+    <row r="176">
+      <c r="A176" t="n">
+        <v>39.06</v>
+      </c>
+      <c r="B176" t="n">
+        <v>0.04000000000000001</v>
+      </c>
+      <c r="C176" t="n">
+        <v>6.611833810806274</v>
+      </c>
+      <c r="D176" t="n">
+        <v>6.375</v>
+      </c>
+    </row>
+    <row r="177">
+      <c r="A177" t="n">
+        <v>39.06</v>
+      </c>
+      <c r="B177" t="n">
+        <v>0.04000000000000001</v>
+      </c>
+      <c r="C177" t="n">
+        <v>5.285555362701416</v>
+      </c>
+      <c r="D177" t="n">
+        <v>5.21875</v>
+      </c>
+    </row>
+    <row r="178">
+      <c r="A178" t="n">
+        <v>39.78</v>
+      </c>
+      <c r="B178" t="n">
+        <v>0.16</v>
+      </c>
+      <c r="C178" t="n">
+        <v>19.69591951370239</v>
+      </c>
+      <c r="D178" t="n">
+        <v>19.578125</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
finished fixing slopes in slopes
</commit_message>
<xml_diff>
--- a/Modules/Main/results.xlsx
+++ b/Modules/Main/results.xlsx
@@ -424,7 +424,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D191"/>
+  <dimension ref="A1:D192"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -3099,6 +3099,20 @@
         <v>31.4375</v>
       </c>
     </row>
+    <row r="192">
+      <c r="A192" t="n">
+        <v>39.06</v>
+      </c>
+      <c r="B192" t="n">
+        <v>0.04000000000000001</v>
+      </c>
+      <c r="C192" t="n">
+        <v>3.896192789077759</v>
+      </c>
+      <c r="D192" t="n">
+        <v>1.09375</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
cleaning constants, still need to fis smooth
</commit_message>
<xml_diff>
--- a/Modules/Main/results.xlsx
+++ b/Modules/Main/results.xlsx
@@ -424,7 +424,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D209"/>
+  <dimension ref="A1:D208"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -3101,16 +3101,16 @@
     </row>
     <row r="192">
       <c r="A192" t="n">
-        <v>39.78</v>
+        <v>39.06</v>
       </c>
       <c r="B192" t="n">
-        <v>0.16</v>
+        <v>0.04000000000000001</v>
       </c>
       <c r="C192" t="n">
-        <v>13.93414235115051</v>
+        <v>3.896192789077759</v>
       </c>
       <c r="D192" t="n">
-        <v>12.546875</v>
+        <v>1.09375</v>
       </c>
     </row>
     <row r="193">
@@ -3121,10 +3121,10 @@
         <v>0.16</v>
       </c>
       <c r="C193" t="n">
-        <v>11.99170398712158</v>
+        <v>10.04770517349243</v>
       </c>
       <c r="D193" t="n">
-        <v>10.953125</v>
+        <v>7.53125</v>
       </c>
     </row>
     <row r="194">
@@ -3135,10 +3135,10 @@
         <v>0.16</v>
       </c>
       <c r="C194" t="n">
-        <v>31.33109641075134</v>
+        <v>23.37266087532043</v>
       </c>
       <c r="D194" t="n">
-        <v>30.0625</v>
+        <v>14.328125</v>
       </c>
     </row>
     <row r="195">
@@ -3149,122 +3149,122 @@
         <v>0.16</v>
       </c>
       <c r="C195" t="n">
-        <v>33.86515688896179</v>
+        <v>23.50989937782288</v>
       </c>
       <c r="D195" t="n">
-        <v>32.59375</v>
+        <v>14.453125</v>
       </c>
     </row>
     <row r="196">
       <c r="A196" t="n">
-        <v>39.78</v>
+        <v>54.5</v>
       </c>
       <c r="B196" t="n">
         <v>0.16</v>
       </c>
       <c r="C196" t="n">
-        <v>24.20807886123657</v>
+        <v>30.71380376815796</v>
       </c>
       <c r="D196" t="n">
-        <v>23</v>
+        <v>18.90625</v>
       </c>
     </row>
     <row r="197">
       <c r="A197" t="n">
-        <v>39.78</v>
+        <v>54.5</v>
       </c>
       <c r="B197" t="n">
         <v>0.16</v>
       </c>
       <c r="C197" t="n">
-        <v>22.04049181938171</v>
+        <v>39.19084405899048</v>
       </c>
       <c r="D197" t="n">
-        <v>21.078125</v>
+        <v>17.96875</v>
       </c>
     </row>
     <row r="198">
       <c r="A198" t="n">
-        <v>39.78</v>
+        <v>39.06</v>
       </c>
       <c r="B198" t="n">
-        <v>0.16</v>
+        <v>0.04000000000000001</v>
       </c>
       <c r="C198" t="n">
-        <v>24.0624475479126</v>
+        <v>6.48872709274292</v>
       </c>
       <c r="D198" t="n">
-        <v>22.703125</v>
+        <v>3.015625</v>
       </c>
     </row>
     <row r="199">
       <c r="A199" t="n">
-        <v>39.78</v>
+        <v>3.6</v>
       </c>
       <c r="B199" t="n">
-        <v>0.16</v>
+        <v>0.04000000000000001</v>
       </c>
       <c r="C199" t="n">
-        <v>21.58569931983948</v>
+        <v>7.816614866256714</v>
       </c>
       <c r="D199" t="n">
-        <v>19.875</v>
+        <v>3.609375</v>
       </c>
     </row>
     <row r="200">
       <c r="A200" t="n">
-        <v>39.78</v>
+        <v>3.6</v>
       </c>
       <c r="B200" t="n">
-        <v>0.16</v>
+        <v>0.04000000000000001</v>
       </c>
       <c r="C200" t="n">
-        <v>33.4221727848053</v>
+        <v>4.427245378494263</v>
       </c>
       <c r="D200" t="n">
-        <v>32.265625</v>
+        <v>2.328125</v>
       </c>
     </row>
     <row r="201">
       <c r="A201" t="n">
-        <v>39.78</v>
+        <v>59.83</v>
       </c>
       <c r="B201" t="n">
-        <v>0.16</v>
+        <v>0.04000000000000001</v>
       </c>
       <c r="C201" t="n">
-        <v>35.24933004379272</v>
+        <v>8.842975854873657</v>
       </c>
       <c r="D201" t="n">
-        <v>33.734375</v>
+        <v>3.484375</v>
       </c>
     </row>
     <row r="202">
       <c r="A202" t="n">
-        <v>39.78</v>
+        <v>39.06</v>
       </c>
       <c r="B202" t="n">
-        <v>0.16</v>
+        <v>0.04000000000000001</v>
       </c>
       <c r="C202" t="n">
-        <v>34.35644316673279</v>
+        <v>103.8992028236389</v>
       </c>
       <c r="D202" t="n">
-        <v>33.03125</v>
+        <v>4.765625</v>
       </c>
     </row>
     <row r="203">
       <c r="A203" t="n">
-        <v>39.78</v>
+        <v>39.06</v>
       </c>
       <c r="B203" t="n">
-        <v>0.16</v>
+        <v>0.04000000000000001</v>
       </c>
       <c r="C203" t="n">
-        <v>30.83824396133423</v>
+        <v>7.417251348495483</v>
       </c>
       <c r="D203" t="n">
-        <v>29.640625</v>
+        <v>2.984375</v>
       </c>
     </row>
     <row r="204">
@@ -3275,10 +3275,10 @@
         <v>0.16</v>
       </c>
       <c r="C204" t="n">
-        <v>38.13737058639526</v>
+        <v>22.68746423721313</v>
       </c>
       <c r="D204" t="n">
-        <v>37.25</v>
+        <v>13.84375</v>
       </c>
     </row>
     <row r="205">
@@ -3289,38 +3289,38 @@
         <v>0.16</v>
       </c>
       <c r="C205" t="n">
-        <v>35.61975622177124</v>
+        <v>43.00482630729675</v>
       </c>
       <c r="D205" t="n">
-        <v>34.046875</v>
+        <v>18.4375</v>
       </c>
     </row>
     <row r="206">
       <c r="A206" t="n">
-        <v>39.78</v>
+        <v>39.06</v>
       </c>
       <c r="B206" t="n">
-        <v>0.16</v>
+        <v>0.04000000000000001</v>
       </c>
       <c r="C206" t="n">
-        <v>38.56909799575806</v>
+        <v>6.663230180740356</v>
       </c>
       <c r="D206" t="n">
-        <v>37.234375</v>
+        <v>3.4375</v>
       </c>
     </row>
     <row r="207">
       <c r="A207" t="n">
-        <v>39.78</v>
+        <v>39.06</v>
       </c>
       <c r="B207" t="n">
-        <v>0.16</v>
+        <v>0.04000000000000001</v>
       </c>
       <c r="C207" t="n">
-        <v>35.97242045402527</v>
+        <v>7.120179891586304</v>
       </c>
       <c r="D207" t="n">
-        <v>34.71875</v>
+        <v>3.390625</v>
       </c>
     </row>
     <row r="208">
@@ -3331,24 +3331,10 @@
         <v>0.16</v>
       </c>
       <c r="C208" t="n">
-        <v>21.42554616928101</v>
+        <v>22.58138370513916</v>
       </c>
       <c r="D208" t="n">
-        <v>20.171875</v>
-      </c>
-    </row>
-    <row r="209">
-      <c r="A209" t="n">
-        <v>39.78</v>
-      </c>
-      <c r="B209" t="n">
-        <v>0.16</v>
-      </c>
-      <c r="C209" t="n">
-        <v>33.86323261260986</v>
-      </c>
-      <c r="D209" t="n">
-        <v>32.71875</v>
+        <v>14.84375</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
shp model almost done
</commit_message>
<xml_diff>
--- a/Modules/Main/results.xlsx
+++ b/Modules/Main/results.xlsx
@@ -424,7 +424,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D212"/>
+  <dimension ref="A1:D213"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -3393,6 +3393,20 @@
         <v>23.125</v>
       </c>
     </row>
+    <row r="213">
+      <c r="A213" t="n">
+        <v>39.78</v>
+      </c>
+      <c r="B213" t="n">
+        <v>0.16</v>
+      </c>
+      <c r="C213" t="n">
+        <v>23.54975008964539</v>
+      </c>
+      <c r="D213" t="n">
+        <v>19.921875</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added inital structure for filter areas
</commit_message>
<xml_diff>
--- a/Modules/Main/results.xlsx
+++ b/Modules/Main/results.xlsx
@@ -424,7 +424,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D165"/>
+  <dimension ref="A1:D170"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -2735,6 +2735,76 @@
         <v>20.671875</v>
       </c>
     </row>
+    <row r="166">
+      <c r="A166" t="n">
+        <v>39.78</v>
+      </c>
+      <c r="B166" t="n">
+        <v>0.16</v>
+      </c>
+      <c r="C166" t="n">
+        <v>21.67134094238281</v>
+      </c>
+      <c r="D166" t="n">
+        <v>14.46875</v>
+      </c>
+    </row>
+    <row r="167">
+      <c r="A167" t="n">
+        <v>39.78</v>
+      </c>
+      <c r="B167" t="n">
+        <v>0.16</v>
+      </c>
+      <c r="C167" t="n">
+        <v>23.73887777328491</v>
+      </c>
+      <c r="D167" t="n">
+        <v>13.015625</v>
+      </c>
+    </row>
+    <row r="168">
+      <c r="A168" t="n">
+        <v>39.78</v>
+      </c>
+      <c r="B168" t="n">
+        <v>0.16</v>
+      </c>
+      <c r="C168" t="n">
+        <v>21.01453614234924</v>
+      </c>
+      <c r="D168" t="n">
+        <v>14.15625</v>
+      </c>
+    </row>
+    <row r="169">
+      <c r="A169" t="n">
+        <v>100</v>
+      </c>
+      <c r="B169" t="n">
+        <v>0.16</v>
+      </c>
+      <c r="C169" t="n">
+        <v>87.42845106124878</v>
+      </c>
+      <c r="D169" t="n">
+        <v>58.21875</v>
+      </c>
+    </row>
+    <row r="170">
+      <c r="A170" t="n">
+        <v>39.78</v>
+      </c>
+      <c r="B170" t="n">
+        <v>0.16</v>
+      </c>
+      <c r="C170" t="n">
+        <v>23.13685536384583</v>
+      </c>
+      <c r="D170" t="n">
+        <v>12.328125</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Fixed smooth function to remove both types of noise, and added typing to Buildings.py
</commit_message>
<xml_diff>
--- a/Modules/Main/results.xlsx
+++ b/Modules/Main/results.xlsx
@@ -424,7 +424,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D213"/>
+  <dimension ref="A1:D214"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -3101,16 +3101,16 @@
     </row>
     <row r="192">
       <c r="A192" t="n">
-        <v>39.78</v>
+        <v>39.06</v>
       </c>
       <c r="B192" t="n">
-        <v>0.16</v>
+        <v>0.04000000000000001</v>
       </c>
       <c r="C192" t="n">
-        <v>13.93414235115051</v>
+        <v>3.896192789077759</v>
       </c>
       <c r="D192" t="n">
-        <v>12.546875</v>
+        <v>1.09375</v>
       </c>
     </row>
     <row r="193">
@@ -3121,10 +3121,10 @@
         <v>0.16</v>
       </c>
       <c r="C193" t="n">
-        <v>11.99170398712158</v>
+        <v>10.04770517349243</v>
       </c>
       <c r="D193" t="n">
-        <v>10.953125</v>
+        <v>7.53125</v>
       </c>
     </row>
     <row r="194">
@@ -3135,10 +3135,10 @@
         <v>0.16</v>
       </c>
       <c r="C194" t="n">
-        <v>31.33109641075134</v>
+        <v>23.37266087532043</v>
       </c>
       <c r="D194" t="n">
-        <v>30.0625</v>
+        <v>14.328125</v>
       </c>
     </row>
     <row r="195">
@@ -3149,122 +3149,122 @@
         <v>0.16</v>
       </c>
       <c r="C195" t="n">
-        <v>33.86515688896179</v>
+        <v>23.50989937782288</v>
       </c>
       <c r="D195" t="n">
-        <v>32.59375</v>
+        <v>14.453125</v>
       </c>
     </row>
     <row r="196">
       <c r="A196" t="n">
-        <v>39.78</v>
+        <v>54.5</v>
       </c>
       <c r="B196" t="n">
         <v>0.16</v>
       </c>
       <c r="C196" t="n">
-        <v>24.20807886123657</v>
+        <v>30.71380376815796</v>
       </c>
       <c r="D196" t="n">
-        <v>23</v>
+        <v>18.90625</v>
       </c>
     </row>
     <row r="197">
       <c r="A197" t="n">
-        <v>39.78</v>
+        <v>54.5</v>
       </c>
       <c r="B197" t="n">
         <v>0.16</v>
       </c>
       <c r="C197" t="n">
-        <v>22.04049181938171</v>
+        <v>39.19084405899048</v>
       </c>
       <c r="D197" t="n">
-        <v>21.078125</v>
+        <v>17.96875</v>
       </c>
     </row>
     <row r="198">
       <c r="A198" t="n">
-        <v>39.78</v>
+        <v>39.06</v>
       </c>
       <c r="B198" t="n">
-        <v>0.16</v>
+        <v>0.04000000000000001</v>
       </c>
       <c r="C198" t="n">
-        <v>24.0624475479126</v>
+        <v>6.48872709274292</v>
       </c>
       <c r="D198" t="n">
-        <v>22.703125</v>
+        <v>3.015625</v>
       </c>
     </row>
     <row r="199">
       <c r="A199" t="n">
-        <v>39.78</v>
+        <v>3.6</v>
       </c>
       <c r="B199" t="n">
-        <v>0.16</v>
+        <v>0.04000000000000001</v>
       </c>
       <c r="C199" t="n">
-        <v>21.58569931983948</v>
+        <v>7.816614866256714</v>
       </c>
       <c r="D199" t="n">
-        <v>19.875</v>
+        <v>3.609375</v>
       </c>
     </row>
     <row r="200">
       <c r="A200" t="n">
-        <v>39.78</v>
+        <v>3.6</v>
       </c>
       <c r="B200" t="n">
-        <v>0.16</v>
+        <v>0.04000000000000001</v>
       </c>
       <c r="C200" t="n">
-        <v>33.4221727848053</v>
+        <v>4.427245378494263</v>
       </c>
       <c r="D200" t="n">
-        <v>32.265625</v>
+        <v>2.328125</v>
       </c>
     </row>
     <row r="201">
       <c r="A201" t="n">
-        <v>39.78</v>
+        <v>59.83</v>
       </c>
       <c r="B201" t="n">
-        <v>0.16</v>
+        <v>0.04000000000000001</v>
       </c>
       <c r="C201" t="n">
-        <v>35.24933004379272</v>
+        <v>8.842975854873657</v>
       </c>
       <c r="D201" t="n">
-        <v>33.734375</v>
+        <v>3.484375</v>
       </c>
     </row>
     <row r="202">
       <c r="A202" t="n">
-        <v>39.78</v>
+        <v>39.06</v>
       </c>
       <c r="B202" t="n">
-        <v>0.16</v>
+        <v>0.04000000000000001</v>
       </c>
       <c r="C202" t="n">
-        <v>34.35644316673279</v>
+        <v>103.8992028236389</v>
       </c>
       <c r="D202" t="n">
-        <v>33.03125</v>
+        <v>4.765625</v>
       </c>
     </row>
     <row r="203">
       <c r="A203" t="n">
-        <v>39.78</v>
+        <v>39.06</v>
       </c>
       <c r="B203" t="n">
-        <v>0.16</v>
+        <v>0.04000000000000001</v>
       </c>
       <c r="C203" t="n">
-        <v>30.83824396133423</v>
+        <v>7.417251348495483</v>
       </c>
       <c r="D203" t="n">
-        <v>29.640625</v>
+        <v>2.984375</v>
       </c>
     </row>
     <row r="204">
@@ -3275,10 +3275,10 @@
         <v>0.16</v>
       </c>
       <c r="C204" t="n">
-        <v>38.13737058639526</v>
+        <v>22.68746423721313</v>
       </c>
       <c r="D204" t="n">
-        <v>37.25</v>
+        <v>13.84375</v>
       </c>
     </row>
     <row r="205">
@@ -3289,38 +3289,38 @@
         <v>0.16</v>
       </c>
       <c r="C205" t="n">
-        <v>35.61975622177124</v>
+        <v>43.00482630729675</v>
       </c>
       <c r="D205" t="n">
-        <v>34.046875</v>
+        <v>18.4375</v>
       </c>
     </row>
     <row r="206">
       <c r="A206" t="n">
-        <v>39.78</v>
+        <v>39.06</v>
       </c>
       <c r="B206" t="n">
-        <v>0.16</v>
+        <v>0.04000000000000001</v>
       </c>
       <c r="C206" t="n">
-        <v>38.56909799575806</v>
+        <v>6.663230180740356</v>
       </c>
       <c r="D206" t="n">
-        <v>37.234375</v>
+        <v>3.4375</v>
       </c>
     </row>
     <row r="207">
       <c r="A207" t="n">
-        <v>39.78</v>
+        <v>39.06</v>
       </c>
       <c r="B207" t="n">
-        <v>0.16</v>
+        <v>0.04000000000000001</v>
       </c>
       <c r="C207" t="n">
-        <v>35.97242045402527</v>
+        <v>7.120179891586304</v>
       </c>
       <c r="D207" t="n">
-        <v>34.71875</v>
+        <v>3.390625</v>
       </c>
     </row>
     <row r="208">
@@ -3331,52 +3331,52 @@
         <v>0.16</v>
       </c>
       <c r="C208" t="n">
-        <v>21.42554616928101</v>
+        <v>22.58138370513916</v>
       </c>
       <c r="D208" t="n">
-        <v>20.171875</v>
+        <v>14.84375</v>
       </c>
     </row>
     <row r="209">
       <c r="A209" t="n">
-        <v>39.78</v>
+        <v>39.06</v>
       </c>
       <c r="B209" t="n">
-        <v>0.16</v>
+        <v>0.04000000000000001</v>
       </c>
       <c r="C209" t="n">
-        <v>33.86323261260986</v>
+        <v>6.986309766769409</v>
       </c>
       <c r="D209" t="n">
-        <v>32.71875</v>
+        <v>3.09375</v>
       </c>
     </row>
     <row r="210">
       <c r="A210" t="n">
-        <v>39.78</v>
+        <v>39.06</v>
       </c>
       <c r="B210" t="n">
-        <v>0.16</v>
+        <v>0.04000000000000001</v>
       </c>
       <c r="C210" t="n">
-        <v>21.1410083770752</v>
+        <v>6.389602184295654</v>
       </c>
       <c r="D210" t="n">
-        <v>19.59375</v>
+        <v>3.15625</v>
       </c>
     </row>
     <row r="211">
       <c r="A211" t="n">
-        <v>39.78</v>
+        <v>39.06</v>
       </c>
       <c r="B211" t="n">
-        <v>0.16</v>
+        <v>0.04000000000000001</v>
       </c>
       <c r="C211" t="n">
-        <v>29.48842597007751</v>
+        <v>6.762027502059937</v>
       </c>
       <c r="D211" t="n">
-        <v>27.203125</v>
+        <v>3.125</v>
       </c>
     </row>
     <row r="212">
@@ -3387,10 +3387,10 @@
         <v>0.16</v>
       </c>
       <c r="C212" t="n">
-        <v>25.18385910987854</v>
+        <v>21.98983311653137</v>
       </c>
       <c r="D212" t="n">
-        <v>23.125</v>
+        <v>15.828125</v>
       </c>
     </row>
     <row r="213">
@@ -3401,10 +3401,24 @@
         <v>0.16</v>
       </c>
       <c r="C213" t="n">
-        <v>23.54975008964539</v>
+        <v>24.83666658401489</v>
       </c>
       <c r="D213" t="n">
-        <v>19.921875</v>
+        <v>9.46875</v>
+      </c>
+    </row>
+    <row r="214">
+      <c r="A214" t="n">
+        <v>39.78</v>
+      </c>
+      <c r="B214" t="n">
+        <v>0.16</v>
+      </c>
+      <c r="C214" t="n">
+        <v>23.77997732162476</v>
+      </c>
+      <c r="D214" t="n">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added a utils file, for generic functions, currently has only the enlarge_obstacles function, imported it from main
</commit_message>
<xml_diff>
--- a/Modules/Main/results.xlsx
+++ b/Modules/Main/results.xlsx
@@ -424,7 +424,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D214"/>
+  <dimension ref="A1:D219"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -3421,6 +3421,76 @@
         <v>11</v>
       </c>
     </row>
+    <row r="215">
+      <c r="A215" t="n">
+        <v>39.06</v>
+      </c>
+      <c r="B215" t="n">
+        <v>0.04000000000000001</v>
+      </c>
+      <c r="C215" t="n">
+        <v>8.919944286346436</v>
+      </c>
+      <c r="D215" t="n">
+        <v>3.40625</v>
+      </c>
+    </row>
+    <row r="216">
+      <c r="A216" t="n">
+        <v>39.78</v>
+      </c>
+      <c r="B216" t="n">
+        <v>0.16</v>
+      </c>
+      <c r="C216" t="n">
+        <v>24.38289165496826</v>
+      </c>
+      <c r="D216" t="n">
+        <v>15.984375</v>
+      </c>
+    </row>
+    <row r="217">
+      <c r="A217" t="n">
+        <v>39.78</v>
+      </c>
+      <c r="B217" t="n">
+        <v>0.16</v>
+      </c>
+      <c r="C217" t="n">
+        <v>25.35724759101868</v>
+      </c>
+      <c r="D217" t="n">
+        <v>13.09375</v>
+      </c>
+    </row>
+    <row r="218">
+      <c r="A218" t="n">
+        <v>39.06</v>
+      </c>
+      <c r="B218" t="n">
+        <v>0.04000000000000001</v>
+      </c>
+      <c r="C218" t="n">
+        <v>6.70301628112793</v>
+      </c>
+      <c r="D218" t="n">
+        <v>3.40625</v>
+      </c>
+    </row>
+    <row r="219">
+      <c r="A219" t="n">
+        <v>39.06</v>
+      </c>
+      <c r="B219" t="n">
+        <v>0.04000000000000001</v>
+      </c>
+      <c r="C219" t="n">
+        <v>7.414100885391235</v>
+      </c>
+      <c r="D219" t="n">
+        <v>2.921875</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
integration of shp model
</commit_message>
<xml_diff>
--- a/Modules/Main/results.xlsx
+++ b/Modules/Main/results.xlsx
@@ -424,7 +424,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D218"/>
+  <dimension ref="A1:D228"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -3477,6 +3477,146 @@
         <v>234.625</v>
       </c>
     </row>
+    <row r="219">
+      <c r="A219" t="n">
+        <v>39.78</v>
+      </c>
+      <c r="B219" t="n">
+        <v>0.16</v>
+      </c>
+      <c r="C219" t="n">
+        <v>31.95371770858765</v>
+      </c>
+      <c r="D219" t="n">
+        <v>30.75</v>
+      </c>
+    </row>
+    <row r="220">
+      <c r="A220" t="n">
+        <v>39.78</v>
+      </c>
+      <c r="B220" t="n">
+        <v>0.16</v>
+      </c>
+      <c r="C220" t="n">
+        <v>22.45127964019775</v>
+      </c>
+      <c r="D220" t="n">
+        <v>20.78125</v>
+      </c>
+    </row>
+    <row r="221">
+      <c r="A221" t="n">
+        <v>96.52</v>
+      </c>
+      <c r="B221" t="n">
+        <v>0.16</v>
+      </c>
+      <c r="C221" t="n">
+        <v>31.34705519676208</v>
+      </c>
+      <c r="D221" t="n">
+        <v>27.953125</v>
+      </c>
+    </row>
+    <row r="222">
+      <c r="A222" t="n">
+        <v>89.04000000000001</v>
+      </c>
+      <c r="B222" t="n">
+        <v>0.6400000000000001</v>
+      </c>
+      <c r="C222" t="n">
+        <v>109.1994066238403</v>
+      </c>
+      <c r="D222" t="n">
+        <v>104.984375</v>
+      </c>
+    </row>
+    <row r="223">
+      <c r="A223" t="n">
+        <v>92.77</v>
+      </c>
+      <c r="B223" t="n">
+        <v>0.16</v>
+      </c>
+      <c r="C223" t="n">
+        <v>44.22820830345154</v>
+      </c>
+      <c r="D223" t="n">
+        <v>43.0625</v>
+      </c>
+    </row>
+    <row r="224">
+      <c r="A224" t="n">
+        <v>96.52</v>
+      </c>
+      <c r="B224" t="n">
+        <v>0.16</v>
+      </c>
+      <c r="C224" t="n">
+        <v>36.44329810142517</v>
+      </c>
+      <c r="D224" t="n">
+        <v>30.71875</v>
+      </c>
+    </row>
+    <row r="225">
+      <c r="A225" t="n">
+        <v>35.37</v>
+      </c>
+      <c r="B225" t="n">
+        <v>0.16</v>
+      </c>
+      <c r="C225" t="n">
+        <v>24.67563581466675</v>
+      </c>
+      <c r="D225" t="n">
+        <v>21.65625</v>
+      </c>
+    </row>
+    <row r="226">
+      <c r="A226" t="n">
+        <v>93.23</v>
+      </c>
+      <c r="B226" t="n">
+        <v>0.16</v>
+      </c>
+      <c r="C226" t="n">
+        <v>31.18767285346985</v>
+      </c>
+      <c r="D226" t="n">
+        <v>25.921875</v>
+      </c>
+    </row>
+    <row r="227">
+      <c r="A227" t="n">
+        <v>39.78</v>
+      </c>
+      <c r="B227" t="n">
+        <v>0.16</v>
+      </c>
+      <c r="C227" t="n">
+        <v>25.54202795028687</v>
+      </c>
+      <c r="D227" t="n">
+        <v>24.078125</v>
+      </c>
+    </row>
+    <row r="228">
+      <c r="A228" t="n">
+        <v>94.28</v>
+      </c>
+      <c r="B228" t="n">
+        <v>0.36</v>
+      </c>
+      <c r="C228" t="n">
+        <v>140.0095384120941</v>
+      </c>
+      <c r="D228" t="n">
+        <v>135.3125</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
update filter areas - now using sweep line algorithm
</commit_message>
<xml_diff>
--- a/Modules/Main/results.xlsx
+++ b/Modules/Main/results.xlsx
@@ -424,7 +424,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D170"/>
+  <dimension ref="A1:D185"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -2805,6 +2805,216 @@
         <v>12.328125</v>
       </c>
     </row>
+    <row r="171">
+      <c r="A171" t="n">
+        <v>39.78</v>
+      </c>
+      <c r="B171" t="n">
+        <v>0.16</v>
+      </c>
+      <c r="C171" t="n">
+        <v>28.40522003173828</v>
+      </c>
+      <c r="D171" t="n">
+        <v>9.0625</v>
+      </c>
+    </row>
+    <row r="172">
+      <c r="A172" t="n">
+        <v>99.67</v>
+      </c>
+      <c r="B172" t="n">
+        <v>0.16</v>
+      </c>
+      <c r="C172" t="n">
+        <v>34.94150567054749</v>
+      </c>
+      <c r="D172" t="n">
+        <v>12.078125</v>
+      </c>
+    </row>
+    <row r="173">
+      <c r="A173" t="n">
+        <v>100</v>
+      </c>
+      <c r="B173" t="n">
+        <v>0.16</v>
+      </c>
+      <c r="C173" t="n">
+        <v>37.01831841468811</v>
+      </c>
+      <c r="D173" t="n">
+        <v>11.4375</v>
+      </c>
+    </row>
+    <row r="174">
+      <c r="A174" t="n">
+        <v>100</v>
+      </c>
+      <c r="B174" t="n">
+        <v>0.16</v>
+      </c>
+      <c r="C174" t="n">
+        <v>34.95767211914062</v>
+      </c>
+      <c r="D174" t="n">
+        <v>10.375</v>
+      </c>
+    </row>
+    <row r="175">
+      <c r="A175" t="n">
+        <v>100</v>
+      </c>
+      <c r="B175" t="n">
+        <v>0.16</v>
+      </c>
+      <c r="C175" t="n">
+        <v>35.74127435684204</v>
+      </c>
+      <c r="D175" t="n">
+        <v>10.84375</v>
+      </c>
+    </row>
+    <row r="176">
+      <c r="A176" t="n">
+        <v>39.78</v>
+      </c>
+      <c r="B176" t="n">
+        <v>0.16</v>
+      </c>
+      <c r="C176" t="n">
+        <v>25.98540353775024</v>
+      </c>
+      <c r="D176" t="n">
+        <v>9.796875</v>
+      </c>
+    </row>
+    <row r="177">
+      <c r="A177" t="n">
+        <v>100</v>
+      </c>
+      <c r="B177" t="n">
+        <v>0.16</v>
+      </c>
+      <c r="C177" t="n">
+        <v>32.43182468414307</v>
+      </c>
+      <c r="D177" t="n">
+        <v>10.359375</v>
+      </c>
+    </row>
+    <row r="178">
+      <c r="A178" t="n">
+        <v>99.87</v>
+      </c>
+      <c r="B178" t="n">
+        <v>0.16</v>
+      </c>
+      <c r="C178" t="n">
+        <v>38.47451686859131</v>
+      </c>
+      <c r="D178" t="n">
+        <v>14.4375</v>
+      </c>
+    </row>
+    <row r="179">
+      <c r="A179" t="n">
+        <v>39.78</v>
+      </c>
+      <c r="B179" t="n">
+        <v>0.16</v>
+      </c>
+      <c r="C179" t="n">
+        <v>26.25908422470093</v>
+      </c>
+      <c r="D179" t="n">
+        <v>9.65625</v>
+      </c>
+    </row>
+    <row r="180">
+      <c r="A180" t="n">
+        <v>100</v>
+      </c>
+      <c r="B180" t="n">
+        <v>0.16</v>
+      </c>
+      <c r="C180" t="n">
+        <v>38.42415428161621</v>
+      </c>
+      <c r="D180" t="n">
+        <v>12.078125</v>
+      </c>
+    </row>
+    <row r="181">
+      <c r="A181" t="n">
+        <v>39.78</v>
+      </c>
+      <c r="B181" t="n">
+        <v>0.16</v>
+      </c>
+      <c r="C181" t="n">
+        <v>25.04115033149719</v>
+      </c>
+      <c r="D181" t="n">
+        <v>8.1875</v>
+      </c>
+    </row>
+    <row r="182">
+      <c r="A182" t="n">
+        <v>98.75</v>
+      </c>
+      <c r="B182" t="n">
+        <v>0.16</v>
+      </c>
+      <c r="C182" t="n">
+        <v>39.76158237457275</v>
+      </c>
+      <c r="D182" t="n">
+        <v>13.71875</v>
+      </c>
+    </row>
+    <row r="183">
+      <c r="A183" t="n">
+        <v>39.78</v>
+      </c>
+      <c r="B183" t="n">
+        <v>0.16</v>
+      </c>
+      <c r="C183" t="n">
+        <v>117.7494630813599</v>
+      </c>
+      <c r="D183" t="n">
+        <v>10.5</v>
+      </c>
+    </row>
+    <row r="184">
+      <c r="A184" t="n">
+        <v>39.78</v>
+      </c>
+      <c r="B184" t="n">
+        <v>0.16</v>
+      </c>
+      <c r="C184" t="n">
+        <v>80.7268750667572</v>
+      </c>
+      <c r="D184" t="n">
+        <v>10.046875</v>
+      </c>
+    </row>
+    <row r="185">
+      <c r="A185" t="n">
+        <v>100</v>
+      </c>
+      <c r="B185" t="n">
+        <v>0.16</v>
+      </c>
+      <c r="C185" t="n">
+        <v>37.93001079559326</v>
+      </c>
+      <c r="D185" t="n">
+        <v>11.265625</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Finalized the filter_chopper_area function, using cv2 dilation via enlarge_obstacles. Moved the previous implementation to legacy
</commit_message>
<xml_diff>
--- a/Modules/Main/results.xlsx
+++ b/Modules/Main/results.xlsx
@@ -424,7 +424,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D219"/>
+  <dimension ref="A1:D223"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -3491,6 +3491,62 @@
         <v>2.921875</v>
       </c>
     </row>
+    <row r="220">
+      <c r="A220" t="n">
+        <v>39.78</v>
+      </c>
+      <c r="B220" t="n">
+        <v>0.16</v>
+      </c>
+      <c r="C220" t="n">
+        <v>23.74857687950134</v>
+      </c>
+      <c r="D220" t="n">
+        <v>16.28125</v>
+      </c>
+    </row>
+    <row r="221">
+      <c r="A221" t="n">
+        <v>39.78</v>
+      </c>
+      <c r="B221" t="n">
+        <v>0.16</v>
+      </c>
+      <c r="C221" t="n">
+        <v>38.82865643501282</v>
+      </c>
+      <c r="D221" t="n">
+        <v>18.640625</v>
+      </c>
+    </row>
+    <row r="222">
+      <c r="A222" t="n">
+        <v>39.78</v>
+      </c>
+      <c r="B222" t="n">
+        <v>0.16</v>
+      </c>
+      <c r="C222" t="n">
+        <v>91.12993431091309</v>
+      </c>
+      <c r="D222" t="n">
+        <v>22.765625</v>
+      </c>
+    </row>
+    <row r="223">
+      <c r="A223" t="n">
+        <v>39.06</v>
+      </c>
+      <c r="B223" t="n">
+        <v>0.04000000000000001</v>
+      </c>
+      <c r="C223" t="n">
+        <v>10.32614302635193</v>
+      </c>
+      <c r="D223" t="n">
+        <v>5.03125</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
start write shp (and delete double filter)
</commit_message>
<xml_diff>
--- a/Modules/Main/results.xlsx
+++ b/Modules/Main/results.xlsx
@@ -424,7 +424,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D228"/>
+  <dimension ref="A1:D242"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -3617,6 +3617,202 @@
         <v>135.3125</v>
       </c>
     </row>
+    <row r="229">
+      <c r="A229" t="n">
+        <v>39.78</v>
+      </c>
+      <c r="B229" t="n">
+        <v>0.16</v>
+      </c>
+      <c r="C229" t="n">
+        <v>43.16329216957092</v>
+      </c>
+      <c r="D229" t="n">
+        <v>40.296875</v>
+      </c>
+    </row>
+    <row r="230">
+      <c r="A230" t="n">
+        <v>37.37</v>
+      </c>
+      <c r="B230" t="n">
+        <v>0.36</v>
+      </c>
+      <c r="C230" t="n">
+        <v>55.52490019798279</v>
+      </c>
+      <c r="D230" t="n">
+        <v>51.75</v>
+      </c>
+    </row>
+    <row r="231">
+      <c r="A231" t="n">
+        <v>39.78</v>
+      </c>
+      <c r="B231" t="n">
+        <v>0.16</v>
+      </c>
+      <c r="C231" t="n">
+        <v>38.23706722259521</v>
+      </c>
+      <c r="D231" t="n">
+        <v>34.296875</v>
+      </c>
+    </row>
+    <row r="232">
+      <c r="A232" t="n">
+        <v>37.37</v>
+      </c>
+      <c r="B232" t="n">
+        <v>0.36</v>
+      </c>
+      <c r="C232" t="n">
+        <v>80.1137330532074</v>
+      </c>
+      <c r="D232" t="n">
+        <v>74.453125</v>
+      </c>
+    </row>
+    <row r="233">
+      <c r="A233" t="n">
+        <v>39.78</v>
+      </c>
+      <c r="B233" t="n">
+        <v>0.16</v>
+      </c>
+      <c r="C233" t="n">
+        <v>23.20184087753296</v>
+      </c>
+      <c r="D233" t="n">
+        <v>20.78125</v>
+      </c>
+    </row>
+    <row r="234">
+      <c r="A234" t="n">
+        <v>66.45999999999999</v>
+      </c>
+      <c r="B234" t="n">
+        <v>0.6400000000000001</v>
+      </c>
+      <c r="C234" t="n">
+        <v>168.7978188991547</v>
+      </c>
+      <c r="D234" t="n">
+        <v>162.71875</v>
+      </c>
+    </row>
+    <row r="235">
+      <c r="A235" t="n">
+        <v>69.63</v>
+      </c>
+      <c r="B235" t="n">
+        <v>0.16</v>
+      </c>
+      <c r="C235" t="n">
+        <v>43.12589979171753</v>
+      </c>
+      <c r="D235" t="n">
+        <v>42.796875</v>
+      </c>
+    </row>
+    <row r="236">
+      <c r="A236" t="n">
+        <v>37.37</v>
+      </c>
+      <c r="B236" t="n">
+        <v>0.36</v>
+      </c>
+      <c r="C236" t="n">
+        <v>82.05421042442322</v>
+      </c>
+      <c r="D236" t="n">
+        <v>80.046875</v>
+      </c>
+    </row>
+    <row r="237">
+      <c r="A237" t="n">
+        <v>39.78</v>
+      </c>
+      <c r="B237" t="n">
+        <v>0.16</v>
+      </c>
+      <c r="C237" t="n">
+        <v>34.1039719581604</v>
+      </c>
+      <c r="D237" t="n">
+        <v>34.140625</v>
+      </c>
+    </row>
+    <row r="238">
+      <c r="A238" t="n">
+        <v>39.78</v>
+      </c>
+      <c r="B238" t="n">
+        <v>0.16</v>
+      </c>
+      <c r="C238" t="n">
+        <v>38.44294476509094</v>
+      </c>
+      <c r="D238" t="n">
+        <v>38.5625</v>
+      </c>
+    </row>
+    <row r="239">
+      <c r="A239" t="n">
+        <v>39.78</v>
+      </c>
+      <c r="B239" t="n">
+        <v>0.16</v>
+      </c>
+      <c r="C239" t="n">
+        <v>38.57809257507324</v>
+      </c>
+      <c r="D239" t="n">
+        <v>38.046875</v>
+      </c>
+    </row>
+    <row r="240">
+      <c r="A240" t="n">
+        <v>39.78</v>
+      </c>
+      <c r="B240" t="n">
+        <v>0.16</v>
+      </c>
+      <c r="C240" t="n">
+        <v>20.44303488731384</v>
+      </c>
+      <c r="D240" t="n">
+        <v>20.359375</v>
+      </c>
+    </row>
+    <row r="241">
+      <c r="A241" t="n">
+        <v>37.37</v>
+      </c>
+      <c r="B241" t="n">
+        <v>0.36</v>
+      </c>
+      <c r="C241" t="n">
+        <v>45.1411452293396</v>
+      </c>
+      <c r="D241" t="n">
+        <v>44.828125</v>
+      </c>
+    </row>
+    <row r="242">
+      <c r="A242" t="n">
+        <v>39.78</v>
+      </c>
+      <c r="B242" t="n">
+        <v>0.16</v>
+      </c>
+      <c r="C242" t="n">
+        <v>28.77275109291077</v>
+      </c>
+      <c r="D242" t="n">
+        <v>28.703125</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Put the filter_chopper_area in main
</commit_message>
<xml_diff>
--- a/Modules/Main/results.xlsx
+++ b/Modules/Main/results.xlsx
@@ -424,7 +424,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D242"/>
+  <dimension ref="A1:D248"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -3813,6 +3813,90 @@
         <v>28.703125</v>
       </c>
     </row>
+    <row r="243">
+      <c r="A243" t="n">
+        <v>39.78</v>
+      </c>
+      <c r="B243" t="n">
+        <v>0.16</v>
+      </c>
+      <c r="C243" t="n">
+        <v>25.83056044578552</v>
+      </c>
+      <c r="D243" t="n">
+        <v>11.53125</v>
+      </c>
+    </row>
+    <row r="244">
+      <c r="A244" t="n">
+        <v>34.57</v>
+      </c>
+      <c r="B244" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="C244" t="n">
+        <v>22.9906702041626</v>
+      </c>
+      <c r="D244" t="n">
+        <v>1.828125</v>
+      </c>
+    </row>
+    <row r="245">
+      <c r="A245" t="n">
+        <v>34.57</v>
+      </c>
+      <c r="B245" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="C245" t="n">
+        <v>3.250611543655396</v>
+      </c>
+      <c r="D245" t="n">
+        <v>0.96875</v>
+      </c>
+    </row>
+    <row r="246">
+      <c r="A246" t="n">
+        <v>39.78</v>
+      </c>
+      <c r="B246" t="n">
+        <v>0.16</v>
+      </c>
+      <c r="C246" t="n">
+        <v>24.17972922325134</v>
+      </c>
+      <c r="D246" t="n">
+        <v>11.859375</v>
+      </c>
+    </row>
+    <row r="247">
+      <c r="A247" t="n">
+        <v>39.78</v>
+      </c>
+      <c r="B247" t="n">
+        <v>0.16</v>
+      </c>
+      <c r="C247" t="n">
+        <v>41.59785151481628</v>
+      </c>
+      <c r="D247" t="n">
+        <v>14.828125</v>
+      </c>
+    </row>
+    <row r="248">
+      <c r="A248" t="n">
+        <v>85.93000000000001</v>
+      </c>
+      <c r="B248" t="n">
+        <v>0.16</v>
+      </c>
+      <c r="C248" t="n">
+        <v>77.33526635169983</v>
+      </c>
+      <c r="D248" t="n">
+        <v>25.734375</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
changed the name of preferences.json, and merges the two functions that get a layer into one
</commit_message>
<xml_diff>
--- a/Modules/Main/results.xlsx
+++ b/Modules/Main/results.xlsx
@@ -424,7 +424,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D248"/>
+  <dimension ref="A1:D253"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -3897,6 +3897,76 @@
         <v>25.734375</v>
       </c>
     </row>
+    <row r="249">
+      <c r="A249" t="n">
+        <v>39.06</v>
+      </c>
+      <c r="B249" t="n">
+        <v>0.04000000000000001</v>
+      </c>
+      <c r="C249" t="n">
+        <v>11.68647933006287</v>
+      </c>
+      <c r="D249" t="n">
+        <v>4.203125</v>
+      </c>
+    </row>
+    <row r="250">
+      <c r="A250" t="n">
+        <v>6.09</v>
+      </c>
+      <c r="B250" t="n">
+        <v>0.04000000000000001</v>
+      </c>
+      <c r="C250" t="n">
+        <v>9.145987272262573</v>
+      </c>
+      <c r="D250" t="n">
+        <v>1.953125</v>
+      </c>
+    </row>
+    <row r="251">
+      <c r="A251" t="n">
+        <v>38.99</v>
+      </c>
+      <c r="B251" t="n">
+        <v>0.16</v>
+      </c>
+      <c r="C251" t="n">
+        <v>59.0127477645874</v>
+      </c>
+      <c r="D251" t="n">
+        <v>18.4375</v>
+      </c>
+    </row>
+    <row r="252">
+      <c r="A252" t="n">
+        <v>39.06</v>
+      </c>
+      <c r="B252" t="n">
+        <v>0.04000000000000001</v>
+      </c>
+      <c r="C252" t="n">
+        <v>12.74627947807312</v>
+      </c>
+      <c r="D252" t="n">
+        <v>4.46875</v>
+      </c>
+    </row>
+    <row r="253">
+      <c r="A253" t="n">
+        <v>39.78</v>
+      </c>
+      <c r="B253" t="n">
+        <v>0.16</v>
+      </c>
+      <c r="C253" t="n">
+        <v>52.52869915962219</v>
+      </c>
+      <c r="D253" t="n">
+        <v>19.015625</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
update part of gui and fix speed run in main
</commit_message>
<xml_diff>
--- a/Modules/Main/results.xlsx
+++ b/Modules/Main/results.xlsx
@@ -424,7 +424,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D253"/>
+  <dimension ref="A1:D247"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -3821,38 +3821,38 @@
         <v>0.16</v>
       </c>
       <c r="C243" t="n">
-        <v>25.83056044578552</v>
+        <v>31.28546357154846</v>
       </c>
       <c r="D243" t="n">
-        <v>11.53125</v>
+        <v>27.65625</v>
       </c>
     </row>
     <row r="244">
       <c r="A244" t="n">
-        <v>34.57</v>
+        <v>82.45</v>
       </c>
       <c r="B244" t="n">
-        <v>0.01</v>
+        <v>0.16</v>
       </c>
       <c r="C244" t="n">
-        <v>22.9906702041626</v>
+        <v>41.23247504234314</v>
       </c>
       <c r="D244" t="n">
-        <v>1.828125</v>
+        <v>38.109375</v>
       </c>
     </row>
     <row r="245">
       <c r="A245" t="n">
-        <v>34.57</v>
+        <v>39.78</v>
       </c>
       <c r="B245" t="n">
-        <v>0.01</v>
+        <v>0.16</v>
       </c>
       <c r="C245" t="n">
-        <v>3.250611543655396</v>
+        <v>37.43526697158813</v>
       </c>
       <c r="D245" t="n">
-        <v>0.96875</v>
+        <v>36.25</v>
       </c>
     </row>
     <row r="246">
@@ -3863,10 +3863,10 @@
         <v>0.16</v>
       </c>
       <c r="C246" t="n">
-        <v>24.17972922325134</v>
+        <v>34.47661805152893</v>
       </c>
       <c r="D246" t="n">
-        <v>11.859375</v>
+        <v>33.0625</v>
       </c>
     </row>
     <row r="247">
@@ -3877,94 +3877,10 @@
         <v>0.16</v>
       </c>
       <c r="C247" t="n">
-        <v>41.59785151481628</v>
+        <v>27.1760106086731</v>
       </c>
       <c r="D247" t="n">
-        <v>14.828125</v>
-      </c>
-    </row>
-    <row r="248">
-      <c r="A248" t="n">
-        <v>85.93000000000001</v>
-      </c>
-      <c r="B248" t="n">
-        <v>0.16</v>
-      </c>
-      <c r="C248" t="n">
-        <v>77.33526635169983</v>
-      </c>
-      <c r="D248" t="n">
-        <v>25.734375</v>
-      </c>
-    </row>
-    <row r="249">
-      <c r="A249" t="n">
-        <v>39.06</v>
-      </c>
-      <c r="B249" t="n">
-        <v>0.04000000000000001</v>
-      </c>
-      <c r="C249" t="n">
-        <v>11.68647933006287</v>
-      </c>
-      <c r="D249" t="n">
-        <v>4.203125</v>
-      </c>
-    </row>
-    <row r="250">
-      <c r="A250" t="n">
-        <v>6.09</v>
-      </c>
-      <c r="B250" t="n">
-        <v>0.04000000000000001</v>
-      </c>
-      <c r="C250" t="n">
-        <v>9.145987272262573</v>
-      </c>
-      <c r="D250" t="n">
-        <v>1.953125</v>
-      </c>
-    </row>
-    <row r="251">
-      <c r="A251" t="n">
-        <v>38.99</v>
-      </c>
-      <c r="B251" t="n">
-        <v>0.16</v>
-      </c>
-      <c r="C251" t="n">
-        <v>59.0127477645874</v>
-      </c>
-      <c r="D251" t="n">
-        <v>18.4375</v>
-      </c>
-    </row>
-    <row r="252">
-      <c r="A252" t="n">
-        <v>39.06</v>
-      </c>
-      <c r="B252" t="n">
-        <v>0.04000000000000001</v>
-      </c>
-      <c r="C252" t="n">
-        <v>12.74627947807312</v>
-      </c>
-      <c r="D252" t="n">
-        <v>4.46875</v>
-      </c>
-    </row>
-    <row r="253">
-      <c r="A253" t="n">
-        <v>39.78</v>
-      </c>
-      <c r="B253" t="n">
-        <v>0.16</v>
-      </c>
-      <c r="C253" t="n">
-        <v>52.52869915962219</v>
-      </c>
-      <c r="D253" t="n">
-        <v>19.015625</v>
+        <v>25.6875</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
modified the stretch and overlay functions to only take a list of masks and a radius
</commit_message>
<xml_diff>
--- a/Modules/Main/results.xlsx
+++ b/Modules/Main/results.xlsx
@@ -424,7 +424,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D247"/>
+  <dimension ref="A1:D264"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -3883,6 +3883,244 @@
         <v>25.6875</v>
       </c>
     </row>
+    <row r="248">
+      <c r="A248" t="n">
+        <v>39.78</v>
+      </c>
+      <c r="B248" t="n">
+        <v>0.16</v>
+      </c>
+      <c r="C248" t="n">
+        <v>23.70307803153992</v>
+      </c>
+      <c r="D248" t="n">
+        <v>17.171875</v>
+      </c>
+    </row>
+    <row r="249">
+      <c r="A249" t="n">
+        <v>37</v>
+      </c>
+      <c r="B249" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="C249" t="n">
+        <v>3.178343534469604</v>
+      </c>
+      <c r="D249" t="n">
+        <v>1.640625</v>
+      </c>
+    </row>
+    <row r="250">
+      <c r="A250" t="n">
+        <v>50</v>
+      </c>
+      <c r="B250" t="n">
+        <v>0.0016</v>
+      </c>
+      <c r="C250" t="n">
+        <v>2.165600299835205</v>
+      </c>
+      <c r="D250" t="n">
+        <v>1.40625</v>
+      </c>
+    </row>
+    <row r="251">
+      <c r="A251" t="n">
+        <v>50</v>
+      </c>
+      <c r="B251" t="n">
+        <v>0.0016</v>
+      </c>
+      <c r="C251" t="n">
+        <v>12.8171751499176</v>
+      </c>
+      <c r="D251" t="n">
+        <v>1.453125</v>
+      </c>
+    </row>
+    <row r="252">
+      <c r="A252" t="n">
+        <v>50</v>
+      </c>
+      <c r="B252" t="n">
+        <v>0.0016</v>
+      </c>
+      <c r="C252" t="n">
+        <v>1.738581657409668</v>
+      </c>
+      <c r="D252" t="n">
+        <v>0.53125</v>
+      </c>
+    </row>
+    <row r="253">
+      <c r="A253" t="n">
+        <v>75</v>
+      </c>
+      <c r="B253" t="n">
+        <v>0.0004</v>
+      </c>
+      <c r="C253" t="n">
+        <v>74.63529062271118</v>
+      </c>
+      <c r="D253" t="n">
+        <v>0.828125</v>
+      </c>
+    </row>
+    <row r="254">
+      <c r="A254" t="n">
+        <v>39.44</v>
+      </c>
+      <c r="B254" t="n">
+        <v>0.16</v>
+      </c>
+      <c r="C254" t="n">
+        <v>30.566237449646</v>
+      </c>
+      <c r="D254" t="n">
+        <v>20.5625</v>
+      </c>
+    </row>
+    <row r="255">
+      <c r="A255" t="n">
+        <v>39.44</v>
+      </c>
+      <c r="B255" t="n">
+        <v>0.16</v>
+      </c>
+      <c r="C255" t="n">
+        <v>23.24444532394409</v>
+      </c>
+      <c r="D255" t="n">
+        <v>18.25</v>
+      </c>
+    </row>
+    <row r="256">
+      <c r="A256" t="n">
+        <v>75</v>
+      </c>
+      <c r="B256" t="n">
+        <v>0.0004</v>
+      </c>
+      <c r="C256" t="n">
+        <v>1.669373512268066</v>
+      </c>
+      <c r="D256" t="n">
+        <v>0.53125</v>
+      </c>
+    </row>
+    <row r="257">
+      <c r="A257" t="n">
+        <v>39.44</v>
+      </c>
+      <c r="B257" t="n">
+        <v>0.16</v>
+      </c>
+      <c r="C257" t="n">
+        <v>21.29177212715149</v>
+      </c>
+      <c r="D257" t="n">
+        <v>15.109375</v>
+      </c>
+    </row>
+    <row r="258">
+      <c r="A258" t="n">
+        <v>39.44</v>
+      </c>
+      <c r="B258" t="n">
+        <v>0.16</v>
+      </c>
+      <c r="C258" t="n">
+        <v>21.79749274253845</v>
+      </c>
+      <c r="D258" t="n">
+        <v>14.71875</v>
+      </c>
+    </row>
+    <row r="259">
+      <c r="A259" t="n">
+        <v>50</v>
+      </c>
+      <c r="B259" t="n">
+        <v>0.0016</v>
+      </c>
+      <c r="C259" t="n">
+        <v>2.104458570480347</v>
+      </c>
+      <c r="D259" t="n">
+        <v>0.875</v>
+      </c>
+    </row>
+    <row r="260">
+      <c r="A260" t="n">
+        <v>75</v>
+      </c>
+      <c r="B260" t="n">
+        <v>0.0004</v>
+      </c>
+      <c r="C260" t="n">
+        <v>1.485002517700195</v>
+      </c>
+      <c r="D260" t="n">
+        <v>0.46875</v>
+      </c>
+    </row>
+    <row r="261">
+      <c r="A261" t="n">
+        <v>33.33</v>
+      </c>
+      <c r="B261" t="n">
+        <v>0.0036</v>
+      </c>
+      <c r="C261" t="n">
+        <v>1.890873670578003</v>
+      </c>
+      <c r="D261" t="n">
+        <v>0.9375</v>
+      </c>
+    </row>
+    <row r="262">
+      <c r="A262" t="n">
+        <v>41.5</v>
+      </c>
+      <c r="B262" t="n">
+        <v>0.04000000000000001</v>
+      </c>
+      <c r="C262" t="n">
+        <v>7.52288556098938</v>
+      </c>
+      <c r="D262" t="n">
+        <v>4.3125</v>
+      </c>
+    </row>
+    <row r="263">
+      <c r="A263" t="n">
+        <v>41.5</v>
+      </c>
+      <c r="B263" t="n">
+        <v>0.04000000000000001</v>
+      </c>
+      <c r="C263" t="n">
+        <v>7.478296279907227</v>
+      </c>
+      <c r="D263" t="n">
+        <v>3.484375</v>
+      </c>
+    </row>
+    <row r="264">
+      <c r="A264" t="n">
+        <v>41.5</v>
+      </c>
+      <c r="B264" t="n">
+        <v>0.04000000000000001</v>
+      </c>
+      <c r="C264" t="n">
+        <v>9.29134726524353</v>
+      </c>
+      <c r="D264" t="n">
+        <v>4.53125</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
removed any other function from main to utils.py
</commit_message>
<xml_diff>
--- a/Modules/Main/results.xlsx
+++ b/Modules/Main/results.xlsx
@@ -424,7 +424,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D264"/>
+  <dimension ref="A1:D266"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -4121,6 +4121,34 @@
         <v>4.53125</v>
       </c>
     </row>
+    <row r="265">
+      <c r="A265" t="n">
+        <v>39.44</v>
+      </c>
+      <c r="B265" t="n">
+        <v>0.16</v>
+      </c>
+      <c r="C265" t="n">
+        <v>53.53329634666443</v>
+      </c>
+      <c r="D265" t="n">
+        <v>19.53125</v>
+      </c>
+    </row>
+    <row r="266">
+      <c r="A266" t="n">
+        <v>26.12</v>
+      </c>
+      <c r="B266" t="n">
+        <v>0.16</v>
+      </c>
+      <c r="C266" t="n">
+        <v>48.22412586212158</v>
+      </c>
+      <c r="D266" t="n">
+        <v>17.203125</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
write_shp.py and doc for read
</commit_message>
<xml_diff>
--- a/Modules/Main/results.xlsx
+++ b/Modules/Main/results.xlsx
@@ -424,7 +424,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D266"/>
+  <dimension ref="A1:D271"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -3885,240 +3885,240 @@
     </row>
     <row r="248">
       <c r="A248" t="n">
-        <v>39.78</v>
+        <v>37.37</v>
       </c>
       <c r="B248" t="n">
-        <v>0.16</v>
+        <v>0.36</v>
       </c>
       <c r="C248" t="n">
-        <v>23.70307803153992</v>
+        <v>46.93020009994507</v>
       </c>
       <c r="D248" t="n">
-        <v>17.171875</v>
+        <v>43.59375</v>
       </c>
     </row>
     <row r="249">
       <c r="A249" t="n">
-        <v>37</v>
+        <v>39.78</v>
       </c>
       <c r="B249" t="n">
-        <v>0.01</v>
+        <v>0.16</v>
       </c>
       <c r="C249" t="n">
-        <v>3.178343534469604</v>
+        <v>49.49240255355835</v>
       </c>
       <c r="D249" t="n">
-        <v>1.640625</v>
+        <v>43.890625</v>
       </c>
     </row>
     <row r="250">
       <c r="A250" t="n">
-        <v>50</v>
+        <v>39.78</v>
       </c>
       <c r="B250" t="n">
-        <v>0.0016</v>
+        <v>0.16</v>
       </c>
       <c r="C250" t="n">
-        <v>2.165600299835205</v>
+        <v>21.56492757797241</v>
       </c>
       <c r="D250" t="n">
-        <v>1.40625</v>
+        <v>21.578125</v>
       </c>
     </row>
     <row r="251">
       <c r="A251" t="n">
-        <v>50</v>
+        <v>39.78</v>
       </c>
       <c r="B251" t="n">
-        <v>0.0016</v>
+        <v>0.16</v>
       </c>
       <c r="C251" t="n">
-        <v>12.8171751499176</v>
+        <v>26.69873666763306</v>
       </c>
       <c r="D251" t="n">
-        <v>1.453125</v>
+        <v>25.03125</v>
       </c>
     </row>
     <row r="252">
       <c r="A252" t="n">
-        <v>50</v>
+        <v>39.44</v>
       </c>
       <c r="B252" t="n">
-        <v>0.0016</v>
+        <v>0.16</v>
       </c>
       <c r="C252" t="n">
-        <v>1.738581657409668</v>
+        <v>26.0681004524231</v>
       </c>
       <c r="D252" t="n">
-        <v>0.53125</v>
+        <v>24.421875</v>
       </c>
     </row>
     <row r="253">
       <c r="A253" t="n">
-        <v>75</v>
+        <v>29.44</v>
       </c>
       <c r="B253" t="n">
-        <v>0.0004</v>
+        <v>0.16</v>
       </c>
       <c r="C253" t="n">
-        <v>74.63529062271118</v>
+        <v>35.41032290458679</v>
       </c>
       <c r="D253" t="n">
-        <v>0.828125</v>
+        <v>31.734375</v>
       </c>
     </row>
     <row r="254">
       <c r="A254" t="n">
-        <v>39.44</v>
+        <v>100</v>
       </c>
       <c r="B254" t="n">
         <v>0.16</v>
       </c>
       <c r="C254" t="n">
-        <v>30.566237449646</v>
+        <v>38.95937848091125</v>
       </c>
       <c r="D254" t="n">
-        <v>20.5625</v>
+        <v>34.53125</v>
       </c>
     </row>
     <row r="255">
       <c r="A255" t="n">
-        <v>39.44</v>
+        <v>23.89</v>
       </c>
       <c r="B255" t="n">
-        <v>0.16</v>
+        <v>0.36</v>
       </c>
       <c r="C255" t="n">
-        <v>23.24444532394409</v>
+        <v>68.09541749954224</v>
       </c>
       <c r="D255" t="n">
-        <v>18.25</v>
+        <v>61.390625</v>
       </c>
     </row>
     <row r="256">
       <c r="A256" t="n">
-        <v>75</v>
+        <v>16.61</v>
       </c>
       <c r="B256" t="n">
-        <v>0.0004</v>
+        <v>0.36</v>
       </c>
       <c r="C256" t="n">
-        <v>1.669373512268066</v>
+        <v>43.96134662628174</v>
       </c>
       <c r="D256" t="n">
-        <v>0.53125</v>
+        <v>40.328125</v>
       </c>
     </row>
     <row r="257">
       <c r="A257" t="n">
-        <v>39.44</v>
+        <v>19.12</v>
       </c>
       <c r="B257" t="n">
         <v>0.16</v>
       </c>
       <c r="C257" t="n">
-        <v>21.29177212715149</v>
+        <v>34.96498870849609</v>
       </c>
       <c r="D257" t="n">
-        <v>15.109375</v>
+        <v>33.15625</v>
       </c>
     </row>
     <row r="258">
       <c r="A258" t="n">
-        <v>39.44</v>
+        <v>75</v>
       </c>
       <c r="B258" t="n">
-        <v>0.16</v>
+        <v>0.0004</v>
       </c>
       <c r="C258" t="n">
-        <v>21.79749274253845</v>
+        <v>1.809213399887085</v>
       </c>
       <c r="D258" t="n">
-        <v>14.71875</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="259">
       <c r="A259" t="n">
-        <v>50</v>
+        <v>75</v>
       </c>
       <c r="B259" t="n">
-        <v>0.0016</v>
+        <v>0.0004</v>
       </c>
       <c r="C259" t="n">
-        <v>2.104458570480347</v>
+        <v>1.765857219696045</v>
       </c>
       <c r="D259" t="n">
-        <v>0.875</v>
+        <v>1.375</v>
       </c>
     </row>
     <row r="260">
       <c r="A260" t="n">
-        <v>75</v>
+        <v>39.44</v>
       </c>
       <c r="B260" t="n">
-        <v>0.0004</v>
+        <v>0.16</v>
       </c>
       <c r="C260" t="n">
-        <v>1.485002517700195</v>
+        <v>41.00721597671509</v>
       </c>
       <c r="D260" t="n">
-        <v>0.46875</v>
+        <v>39.75</v>
       </c>
     </row>
     <row r="261">
       <c r="A261" t="n">
-        <v>33.33</v>
+        <v>37.67</v>
       </c>
       <c r="B261" t="n">
-        <v>0.0036</v>
+        <v>0.36</v>
       </c>
       <c r="C261" t="n">
-        <v>1.890873670578003</v>
+        <v>58.08780217170715</v>
       </c>
       <c r="D261" t="n">
-        <v>0.9375</v>
+        <v>54.03125</v>
       </c>
     </row>
     <row r="262">
       <c r="A262" t="n">
-        <v>41.5</v>
+        <v>37.67</v>
       </c>
       <c r="B262" t="n">
-        <v>0.04000000000000001</v>
+        <v>0.36</v>
       </c>
       <c r="C262" t="n">
-        <v>7.52288556098938</v>
+        <v>69.58404088020325</v>
       </c>
       <c r="D262" t="n">
-        <v>4.3125</v>
+        <v>67.546875</v>
       </c>
     </row>
     <row r="263">
       <c r="A263" t="n">
-        <v>41.5</v>
+        <v>39.44</v>
       </c>
       <c r="B263" t="n">
-        <v>0.04000000000000001</v>
+        <v>0.16</v>
       </c>
       <c r="C263" t="n">
-        <v>7.478296279907227</v>
+        <v>47.34826254844666</v>
       </c>
       <c r="D263" t="n">
-        <v>3.484375</v>
+        <v>45.734375</v>
       </c>
     </row>
     <row r="264">
       <c r="A264" t="n">
-        <v>41.5</v>
+        <v>39.44</v>
       </c>
       <c r="B264" t="n">
-        <v>0.04000000000000001</v>
+        <v>0.16</v>
       </c>
       <c r="C264" t="n">
-        <v>9.29134726524353</v>
+        <v>49.34514284133911</v>
       </c>
       <c r="D264" t="n">
-        <v>4.53125</v>
+        <v>47.875</v>
       </c>
     </row>
     <row r="265">
@@ -4129,24 +4129,94 @@
         <v>0.16</v>
       </c>
       <c r="C265" t="n">
-        <v>53.53329634666443</v>
+        <v>44.41006135940552</v>
       </c>
       <c r="D265" t="n">
-        <v>19.53125</v>
+        <v>42.953125</v>
       </c>
     </row>
     <row r="266">
       <c r="A266" t="n">
-        <v>26.12</v>
+        <v>37</v>
       </c>
       <c r="B266" t="n">
-        <v>0.16</v>
+        <v>0.01</v>
       </c>
       <c r="C266" t="n">
-        <v>48.22412586212158</v>
+        <v>3.879632472991943</v>
       </c>
       <c r="D266" t="n">
-        <v>17.203125</v>
+        <v>2.890625</v>
+      </c>
+    </row>
+    <row r="267">
+      <c r="A267" t="n">
+        <v>75</v>
+      </c>
+      <c r="B267" t="n">
+        <v>0.0004</v>
+      </c>
+      <c r="C267" t="n">
+        <v>2.40252685546875</v>
+      </c>
+      <c r="D267" t="n">
+        <v>2.09375</v>
+      </c>
+    </row>
+    <row r="268">
+      <c r="A268" t="n">
+        <v>50</v>
+      </c>
+      <c r="B268" t="n">
+        <v>0.0016</v>
+      </c>
+      <c r="C268" t="n">
+        <v>2.566594839096069</v>
+      </c>
+      <c r="D268" t="n">
+        <v>2.09375</v>
+      </c>
+    </row>
+    <row r="269">
+      <c r="A269" t="n">
+        <v>39.44</v>
+      </c>
+      <c r="B269" t="n">
+        <v>0.16</v>
+      </c>
+      <c r="C269" t="n">
+        <v>36.68801498413086</v>
+      </c>
+      <c r="D269" t="n">
+        <v>35.109375</v>
+      </c>
+    </row>
+    <row r="270">
+      <c r="A270" t="n">
+        <v>37.67</v>
+      </c>
+      <c r="B270" t="n">
+        <v>0.36</v>
+      </c>
+      <c r="C270" t="n">
+        <v>52.79992604255676</v>
+      </c>
+      <c r="D270" t="n">
+        <v>51.234375</v>
+      </c>
+    </row>
+    <row r="271">
+      <c r="A271" t="n">
+        <v>75</v>
+      </c>
+      <c r="B271" t="n">
+        <v>0.0004</v>
+      </c>
+      <c r="C271" t="n">
+        <v>1.868182420730591</v>
+      </c>
+      <c r="D271" t="n">
+        <v>1.390625</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Initial modifications to make the project split into front and back end
</commit_message>
<xml_diff>
--- a/Modules/Main/results.xlsx
+++ b/Modules/Main/results.xlsx
@@ -424,7 +424,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D271"/>
+  <dimension ref="A1:D294"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -3885,240 +3885,240 @@
     </row>
     <row r="248">
       <c r="A248" t="n">
-        <v>37.37</v>
+        <v>39.78</v>
       </c>
       <c r="B248" t="n">
-        <v>0.36</v>
+        <v>0.16</v>
       </c>
       <c r="C248" t="n">
-        <v>46.93020009994507</v>
+        <v>23.70307803153992</v>
       </c>
       <c r="D248" t="n">
-        <v>43.59375</v>
+        <v>17.171875</v>
       </c>
     </row>
     <row r="249">
       <c r="A249" t="n">
-        <v>39.78</v>
+        <v>37</v>
       </c>
       <c r="B249" t="n">
-        <v>0.16</v>
+        <v>0.01</v>
       </c>
       <c r="C249" t="n">
-        <v>49.49240255355835</v>
+        <v>3.178343534469604</v>
       </c>
       <c r="D249" t="n">
-        <v>43.890625</v>
+        <v>1.640625</v>
       </c>
     </row>
     <row r="250">
       <c r="A250" t="n">
-        <v>39.78</v>
+        <v>50</v>
       </c>
       <c r="B250" t="n">
-        <v>0.16</v>
+        <v>0.0016</v>
       </c>
       <c r="C250" t="n">
-        <v>21.56492757797241</v>
+        <v>2.165600299835205</v>
       </c>
       <c r="D250" t="n">
-        <v>21.578125</v>
+        <v>1.40625</v>
       </c>
     </row>
     <row r="251">
       <c r="A251" t="n">
-        <v>39.78</v>
+        <v>50</v>
       </c>
       <c r="B251" t="n">
-        <v>0.16</v>
+        <v>0.0016</v>
       </c>
       <c r="C251" t="n">
-        <v>26.69873666763306</v>
+        <v>12.8171751499176</v>
       </c>
       <c r="D251" t="n">
-        <v>25.03125</v>
+        <v>1.453125</v>
       </c>
     </row>
     <row r="252">
       <c r="A252" t="n">
-        <v>39.44</v>
+        <v>50</v>
       </c>
       <c r="B252" t="n">
-        <v>0.16</v>
+        <v>0.0016</v>
       </c>
       <c r="C252" t="n">
-        <v>26.0681004524231</v>
+        <v>1.738581657409668</v>
       </c>
       <c r="D252" t="n">
-        <v>24.421875</v>
+        <v>0.53125</v>
       </c>
     </row>
     <row r="253">
       <c r="A253" t="n">
-        <v>29.44</v>
+        <v>75</v>
       </c>
       <c r="B253" t="n">
-        <v>0.16</v>
+        <v>0.0004</v>
       </c>
       <c r="C253" t="n">
-        <v>35.41032290458679</v>
+        <v>74.63529062271118</v>
       </c>
       <c r="D253" t="n">
-        <v>31.734375</v>
+        <v>0.828125</v>
       </c>
     </row>
     <row r="254">
       <c r="A254" t="n">
-        <v>100</v>
+        <v>39.44</v>
       </c>
       <c r="B254" t="n">
         <v>0.16</v>
       </c>
       <c r="C254" t="n">
-        <v>38.95937848091125</v>
+        <v>30.566237449646</v>
       </c>
       <c r="D254" t="n">
-        <v>34.53125</v>
+        <v>20.5625</v>
       </c>
     </row>
     <row r="255">
       <c r="A255" t="n">
-        <v>23.89</v>
+        <v>39.44</v>
       </c>
       <c r="B255" t="n">
-        <v>0.36</v>
+        <v>0.16</v>
       </c>
       <c r="C255" t="n">
-        <v>68.09541749954224</v>
+        <v>23.24444532394409</v>
       </c>
       <c r="D255" t="n">
-        <v>61.390625</v>
+        <v>18.25</v>
       </c>
     </row>
     <row r="256">
       <c r="A256" t="n">
-        <v>16.61</v>
+        <v>75</v>
       </c>
       <c r="B256" t="n">
-        <v>0.36</v>
+        <v>0.0004</v>
       </c>
       <c r="C256" t="n">
-        <v>43.96134662628174</v>
+        <v>1.669373512268066</v>
       </c>
       <c r="D256" t="n">
-        <v>40.328125</v>
+        <v>0.53125</v>
       </c>
     </row>
     <row r="257">
       <c r="A257" t="n">
-        <v>19.12</v>
+        <v>39.44</v>
       </c>
       <c r="B257" t="n">
         <v>0.16</v>
       </c>
       <c r="C257" t="n">
-        <v>34.96498870849609</v>
+        <v>21.29177212715149</v>
       </c>
       <c r="D257" t="n">
-        <v>33.15625</v>
+        <v>15.109375</v>
       </c>
     </row>
     <row r="258">
       <c r="A258" t="n">
-        <v>75</v>
+        <v>39.44</v>
       </c>
       <c r="B258" t="n">
-        <v>0.0004</v>
+        <v>0.16</v>
       </c>
       <c r="C258" t="n">
-        <v>1.809213399887085</v>
+        <v>21.79749274253845</v>
       </c>
       <c r="D258" t="n">
-        <v>1.5</v>
+        <v>14.71875</v>
       </c>
     </row>
     <row r="259">
       <c r="A259" t="n">
-        <v>75</v>
+        <v>50</v>
       </c>
       <c r="B259" t="n">
-        <v>0.0004</v>
+        <v>0.0016</v>
       </c>
       <c r="C259" t="n">
-        <v>1.765857219696045</v>
+        <v>2.104458570480347</v>
       </c>
       <c r="D259" t="n">
-        <v>1.375</v>
+        <v>0.875</v>
       </c>
     </row>
     <row r="260">
       <c r="A260" t="n">
-        <v>39.44</v>
+        <v>75</v>
       </c>
       <c r="B260" t="n">
-        <v>0.16</v>
+        <v>0.0004</v>
       </c>
       <c r="C260" t="n">
-        <v>41.00721597671509</v>
+        <v>1.485002517700195</v>
       </c>
       <c r="D260" t="n">
-        <v>39.75</v>
+        <v>0.46875</v>
       </c>
     </row>
     <row r="261">
       <c r="A261" t="n">
-        <v>37.67</v>
+        <v>33.33</v>
       </c>
       <c r="B261" t="n">
-        <v>0.36</v>
+        <v>0.0036</v>
       </c>
       <c r="C261" t="n">
-        <v>58.08780217170715</v>
+        <v>1.890873670578003</v>
       </c>
       <c r="D261" t="n">
-        <v>54.03125</v>
+        <v>0.9375</v>
       </c>
     </row>
     <row r="262">
       <c r="A262" t="n">
-        <v>37.67</v>
+        <v>41.5</v>
       </c>
       <c r="B262" t="n">
-        <v>0.36</v>
+        <v>0.04000000000000001</v>
       </c>
       <c r="C262" t="n">
-        <v>69.58404088020325</v>
+        <v>7.52288556098938</v>
       </c>
       <c r="D262" t="n">
-        <v>67.546875</v>
+        <v>4.3125</v>
       </c>
     </row>
     <row r="263">
       <c r="A263" t="n">
-        <v>39.44</v>
+        <v>41.5</v>
       </c>
       <c r="B263" t="n">
-        <v>0.16</v>
+        <v>0.04000000000000001</v>
       </c>
       <c r="C263" t="n">
-        <v>47.34826254844666</v>
+        <v>7.478296279907227</v>
       </c>
       <c r="D263" t="n">
-        <v>45.734375</v>
+        <v>3.484375</v>
       </c>
     </row>
     <row r="264">
       <c r="A264" t="n">
-        <v>39.44</v>
+        <v>41.5</v>
       </c>
       <c r="B264" t="n">
-        <v>0.16</v>
+        <v>0.04000000000000001</v>
       </c>
       <c r="C264" t="n">
-        <v>49.34514284133911</v>
+        <v>9.29134726524353</v>
       </c>
       <c r="D264" t="n">
-        <v>47.875</v>
+        <v>4.53125</v>
       </c>
     </row>
     <row r="265">
@@ -4129,94 +4129,416 @@
         <v>0.16</v>
       </c>
       <c r="C265" t="n">
-        <v>44.41006135940552</v>
+        <v>53.53329634666443</v>
       </c>
       <c r="D265" t="n">
-        <v>42.953125</v>
+        <v>19.53125</v>
       </c>
     </row>
     <row r="266">
       <c r="A266" t="n">
-        <v>37</v>
+        <v>26.12</v>
       </c>
       <c r="B266" t="n">
-        <v>0.01</v>
+        <v>0.16</v>
       </c>
       <c r="C266" t="n">
-        <v>3.879632472991943</v>
+        <v>48.22412586212158</v>
       </c>
       <c r="D266" t="n">
-        <v>2.890625</v>
+        <v>17.203125</v>
       </c>
     </row>
     <row r="267">
       <c r="A267" t="n">
-        <v>75</v>
+        <v>40.31</v>
       </c>
       <c r="B267" t="n">
-        <v>0.0004</v>
+        <v>0.0196</v>
       </c>
       <c r="C267" t="n">
-        <v>2.40252685546875</v>
+        <v>4.094011783599854</v>
       </c>
       <c r="D267" t="n">
-        <v>2.09375</v>
+        <v>1.734375</v>
       </c>
     </row>
     <row r="268">
       <c r="A268" t="n">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="B268" t="n">
-        <v>0.0016</v>
+        <v>0.0036</v>
       </c>
       <c r="C268" t="n">
-        <v>2.566594839096069</v>
+        <v>2.080069303512573</v>
       </c>
       <c r="D268" t="n">
-        <v>2.09375</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="269">
       <c r="A269" t="n">
-        <v>39.44</v>
+        <v>0</v>
       </c>
       <c r="B269" t="n">
-        <v>0.16</v>
+        <v>0.0036</v>
       </c>
       <c r="C269" t="n">
-        <v>36.68801498413086</v>
+        <v>2.129308938980103</v>
       </c>
       <c r="D269" t="n">
-        <v>35.109375</v>
+        <v>0.734375</v>
       </c>
     </row>
     <row r="270">
       <c r="A270" t="n">
-        <v>37.67</v>
+        <v>0</v>
       </c>
       <c r="B270" t="n">
-        <v>0.36</v>
+        <v>0.04000000000000001</v>
       </c>
       <c r="C270" t="n">
-        <v>52.79992604255676</v>
+        <v>8.243014097213745</v>
       </c>
       <c r="D270" t="n">
-        <v>51.234375</v>
+        <v>4.21875</v>
       </c>
     </row>
     <row r="271">
       <c r="A271" t="n">
-        <v>75</v>
+        <v>0</v>
       </c>
       <c r="B271" t="n">
-        <v>0.0004</v>
+        <v>0.0016</v>
       </c>
       <c r="C271" t="n">
-        <v>1.868182420730591</v>
+        <v>1.666461706161499</v>
       </c>
       <c r="D271" t="n">
-        <v>1.390625</v>
+        <v>0.84375</v>
+      </c>
+    </row>
+    <row r="272">
+      <c r="A272" t="n">
+        <v>0</v>
+      </c>
+      <c r="B272" t="n">
+        <v>0.0016</v>
+      </c>
+      <c r="C272" t="n">
+        <v>1.679929733276367</v>
+      </c>
+      <c r="D272" t="n">
+        <v>0.921875</v>
+      </c>
+    </row>
+    <row r="273">
+      <c r="A273" t="n">
+        <v>0</v>
+      </c>
+      <c r="B273" t="n">
+        <v>0.0016</v>
+      </c>
+      <c r="C273" t="n">
+        <v>1.69499397277832</v>
+      </c>
+      <c r="D273" t="n">
+        <v>0.828125</v>
+      </c>
+    </row>
+    <row r="274">
+      <c r="A274" t="n">
+        <v>0</v>
+      </c>
+      <c r="B274" t="n">
+        <v>0.0016</v>
+      </c>
+      <c r="C274" t="n">
+        <v>2.639148950576782</v>
+      </c>
+      <c r="D274" t="n">
+        <v>1.453125</v>
+      </c>
+    </row>
+    <row r="275">
+      <c r="A275" t="n">
+        <v>47</v>
+      </c>
+      <c r="B275" t="n">
+        <v>0.0016</v>
+      </c>
+      <c r="C275" t="n">
+        <v>1.721790790557861</v>
+      </c>
+      <c r="D275" t="n">
+        <v>0.796875</v>
+      </c>
+    </row>
+    <row r="276">
+      <c r="A276" t="n">
+        <v>33.25</v>
+      </c>
+      <c r="B276" t="n">
+        <v>0.16</v>
+      </c>
+      <c r="C276" t="n">
+        <v>23.09088778495789</v>
+      </c>
+      <c r="D276" t="n">
+        <v>17.09375</v>
+      </c>
+    </row>
+    <row r="277">
+      <c r="A277" t="n">
+        <v>33.33</v>
+      </c>
+      <c r="B277" t="n">
+        <v>0.04000000000000001</v>
+      </c>
+      <c r="C277" t="n">
+        <v>7.165266036987305</v>
+      </c>
+      <c r="D277" t="n">
+        <v>4.140625</v>
+      </c>
+    </row>
+    <row r="278">
+      <c r="A278" t="n">
+        <v>82.29000000000001</v>
+      </c>
+      <c r="B278" t="n">
+        <v>0.16</v>
+      </c>
+      <c r="C278" t="n">
+        <v>30.96109223365784</v>
+      </c>
+      <c r="D278" t="n">
+        <v>20.359375</v>
+      </c>
+    </row>
+    <row r="279">
+      <c r="A279" t="n">
+        <v>33.25</v>
+      </c>
+      <c r="B279" t="n">
+        <v>0.16</v>
+      </c>
+      <c r="C279" t="n">
+        <v>29.04900670051575</v>
+      </c>
+      <c r="D279" t="n">
+        <v>18.734375</v>
+      </c>
+    </row>
+    <row r="280">
+      <c r="A280" t="n">
+        <v>50.69</v>
+      </c>
+      <c r="B280" t="n">
+        <v>9</v>
+      </c>
+      <c r="C280" t="n">
+        <v>3794.463066339493</v>
+      </c>
+      <c r="D280" t="n">
+        <v>1564.6875</v>
+      </c>
+    </row>
+    <row r="281">
+      <c r="A281" t="n">
+        <v>0.08</v>
+      </c>
+      <c r="B281" t="n">
+        <v>0.04000000000000001</v>
+      </c>
+      <c r="C281" t="n">
+        <v>7.809202671051025</v>
+      </c>
+      <c r="D281" t="n">
+        <v>4.234375</v>
+      </c>
+    </row>
+    <row r="282">
+      <c r="A282" t="n">
+        <v>0.99</v>
+      </c>
+      <c r="B282" t="n">
+        <v>0.16</v>
+      </c>
+      <c r="C282" t="n">
+        <v>20.09047985076904</v>
+      </c>
+      <c r="D282" t="n">
+        <v>14.078125</v>
+      </c>
+    </row>
+    <row r="283">
+      <c r="A283" t="n">
+        <v>5.13</v>
+      </c>
+      <c r="B283" t="n">
+        <v>0.09</v>
+      </c>
+      <c r="C283" t="n">
+        <v>12.30720639228821</v>
+      </c>
+      <c r="D283" t="n">
+        <v>8.640625</v>
+      </c>
+    </row>
+    <row r="284">
+      <c r="A284" t="n">
+        <v>2.83</v>
+      </c>
+      <c r="B284" t="n">
+        <v>0.16</v>
+      </c>
+      <c r="C284" t="n">
+        <v>20.97641086578369</v>
+      </c>
+      <c r="D284" t="n">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="285">
+      <c r="A285" t="n">
+        <v>16.7</v>
+      </c>
+      <c r="B285" t="n">
+        <v>0.16</v>
+      </c>
+      <c r="C285" t="n">
+        <v>23.43800830841064</v>
+      </c>
+      <c r="D285" t="n">
+        <v>14.078125</v>
+      </c>
+    </row>
+    <row r="286">
+      <c r="A286" t="n">
+        <v>12.21</v>
+      </c>
+      <c r="B286" t="n">
+        <v>0.16</v>
+      </c>
+      <c r="C286" t="n">
+        <v>21.96702885627747</v>
+      </c>
+      <c r="D286" t="n">
+        <v>16.3125</v>
+      </c>
+    </row>
+    <row r="287">
+      <c r="A287" t="n">
+        <v>12.21</v>
+      </c>
+      <c r="B287" t="n">
+        <v>0.16</v>
+      </c>
+      <c r="C287" t="n">
+        <v>26.15172576904297</v>
+      </c>
+      <c r="D287" t="n">
+        <v>15.15625</v>
+      </c>
+    </row>
+    <row r="288">
+      <c r="A288" t="n">
+        <v>12.21</v>
+      </c>
+      <c r="B288" t="n">
+        <v>0.16</v>
+      </c>
+      <c r="C288" t="n">
+        <v>71.19786858558655</v>
+      </c>
+      <c r="D288" t="n">
+        <v>11.65625</v>
+      </c>
+    </row>
+    <row r="289">
+      <c r="A289" t="n">
+        <v>12.21</v>
+      </c>
+      <c r="B289" t="n">
+        <v>0.16</v>
+      </c>
+      <c r="C289" t="n">
+        <v>43.66991925239563</v>
+      </c>
+      <c r="D289" t="n">
+        <v>9.484375</v>
+      </c>
+    </row>
+    <row r="290">
+      <c r="A290" t="n">
+        <v>12.21</v>
+      </c>
+      <c r="B290" t="n">
+        <v>0.16</v>
+      </c>
+      <c r="C290" t="n">
+        <v>48.34774827957153</v>
+      </c>
+      <c r="D290" t="n">
+        <v>11.34375</v>
+      </c>
+    </row>
+    <row r="291">
+      <c r="A291" t="n">
+        <v>12.21</v>
+      </c>
+      <c r="B291" t="n">
+        <v>0.16</v>
+      </c>
+      <c r="C291" t="n">
+        <v>45.7321879863739</v>
+      </c>
+      <c r="D291" t="n">
+        <v>10.15625</v>
+      </c>
+    </row>
+    <row r="292">
+      <c r="A292" t="n">
+        <v>12.21</v>
+      </c>
+      <c r="B292" t="n">
+        <v>0.16</v>
+      </c>
+      <c r="C292" t="n">
+        <v>57.39707326889038</v>
+      </c>
+      <c r="D292" t="n">
+        <v>25.328125</v>
+      </c>
+    </row>
+    <row r="293">
+      <c r="A293" t="n">
+        <v>12.21</v>
+      </c>
+      <c r="B293" t="n">
+        <v>0.16</v>
+      </c>
+      <c r="C293" t="n">
+        <v>66.89149522781372</v>
+      </c>
+      <c r="D293" t="n">
+        <v>28.359375</v>
+      </c>
+    </row>
+    <row r="294">
+      <c r="A294" t="n">
+        <v>12.21</v>
+      </c>
+      <c r="B294" t="n">
+        <v>0.16</v>
+      </c>
+      <c r="C294" t="n">
+        <v>41.22408008575439</v>
+      </c>
+      <c r="D294" t="n">
+        <v>18.3125</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
removed todos, fixed typing of coordinates
</commit_message>
<xml_diff>
--- a/Modules/Main/results.xlsx
+++ b/Modules/Main/results.xlsx
@@ -424,7 +424,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D294"/>
+  <dimension ref="A1:D297"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -4541,6 +4541,48 @@
         <v>18.3125</v>
       </c>
     </row>
+    <row r="295">
+      <c r="A295" t="n">
+        <v>12.21</v>
+      </c>
+      <c r="B295" t="n">
+        <v>0.16</v>
+      </c>
+      <c r="C295" t="n">
+        <v>25.24234938621521</v>
+      </c>
+      <c r="D295" t="n">
+        <v>12.03125</v>
+      </c>
+    </row>
+    <row r="296">
+      <c r="A296" t="n">
+        <v>12.21</v>
+      </c>
+      <c r="B296" t="n">
+        <v>0.16</v>
+      </c>
+      <c r="C296" t="n">
+        <v>65.02928471565247</v>
+      </c>
+      <c r="D296" t="n">
+        <v>30.671875</v>
+      </c>
+    </row>
+    <row r="297">
+      <c r="A297" t="n">
+        <v>10.25</v>
+      </c>
+      <c r="B297" t="n">
+        <v>0.16</v>
+      </c>
+      <c r="C297" t="n">
+        <v>21.04346394538879</v>
+      </c>
+      <c r="D297" t="n">
+        <v>8.671875</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
support for running from cmd
</commit_message>
<xml_diff>
--- a/Modules/Main/results.xlsx
+++ b/Modules/Main/results.xlsx
@@ -424,7 +424,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D297"/>
+  <dimension ref="A1:D299"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -4583,6 +4583,34 @@
         <v>8.671875</v>
       </c>
     </row>
+    <row r="298">
+      <c r="A298" t="n">
+        <v>12.21</v>
+      </c>
+      <c r="B298" t="n">
+        <v>0.16</v>
+      </c>
+      <c r="C298" t="n">
+        <v>63.58827042579651</v>
+      </c>
+      <c r="D298" t="n">
+        <v>24.5625</v>
+      </c>
+    </row>
+    <row r="299">
+      <c r="A299" t="n">
+        <v>12.21</v>
+      </c>
+      <c r="B299" t="n">
+        <v>0.16</v>
+      </c>
+      <c r="C299" t="n">
+        <v>79.86849761009216</v>
+      </c>
+      <c r="D299" t="n">
+        <v>29.46875</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
DTM moved to DTM_data
</commit_message>
<xml_diff>
--- a/Modules/Main/results.xlsx
+++ b/Modules/Main/results.xlsx
@@ -424,7 +424,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D299"/>
+  <dimension ref="A1:D300"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -4611,6 +4611,20 @@
         <v>29.46875</v>
       </c>
     </row>
+    <row r="300">
+      <c r="A300" t="n">
+        <v>0.45</v>
+      </c>
+      <c r="B300" t="n">
+        <v>0.04000000000000001</v>
+      </c>
+      <c r="C300" t="n">
+        <v>12.1037290096283</v>
+      </c>
+      <c r="D300" t="n">
+        <v>3.875</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>